<commit_message>
done 90%  with showtime in detail/movie
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\#Lap trinh Web 2\Theory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Exercises\LTWeb2\Đồ Án Cuối Kỳ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51AD78A-5DEA-4DBA-8E6F-EEF2B0F7790A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3769505-F42C-4619-8B0B-2C45113A73F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{EFC861EB-62D1-4F27-80DA-EEC53D8209EB}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" activeTab="3" xr2:uid="{EFC861EB-62D1-4F27-80DA-EEC53D8209EB}"/>
   </bookViews>
   <sheets>
     <sheet name="TheaterCluster" sheetId="1" r:id="rId1"/>
@@ -26,21 +26,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
   <si>
     <t>id</t>
   </si>
@@ -223,6 +214,27 @@
   </si>
   <si>
     <t>\xffd8ffe000104a46494600010101004800480000ffdb004300080606070605080707070909080a0c140d0c0b0b0c1912130f141d1a1f1e1d1a1c1c20242e2720222c231c1c2837292c30313434341f27393d38323c2e333432ffdb0043010909090c0b0c180d0d1832211c213232323232323232323232323232323232323232323232323232323232323232323232323232323232323232323232323232ffc20011080546043803012200021101031101ffc4001b00000203010101000000000000000000000001020304050607ffc4001a010101010101010100000000000000000000010203040506ffda000c03010002100310000001f10cb33d54ec8e76511cfae6e21ae600000000000000000000e758740a218eb6c2eae90163403103040d354020000000c4304c00051348301305001269004834c94a125b4ac87118eda6458e12944ea494aa5538c82034820013b18251a11b109c4499092df6d164b6b8035106ac81546c41224488c8aa37408c2c99956e8191688a52a51a94ea94b71584e1208906592ad922210babb674a2b966bcda0d600000000000000000000000000b6ab25d7569cf9ea935ac800000d0000c128020343014000000000018000818a3248804001b88484137072b6d8826571be810c41808922285636856d0324a1292b14930b54a507222843729098cadd77135070850a9454c96a8116d2ea2b708d5b592235df4918a2c9b84a56ac8906c0261657762cf5a60d74f38000000000000000000000000000005dbf9fd3c76c95e8cf6005800000035040008d30005000681a189840000002624ca88d20022681b41294652db1224e7484e0810c473aec57120463257200306b26295c64224e24ca99a259a44dca44a55c967102a958a21150b2708a2dbe899a239e51695aa9d1732a5a2267534531b048c88974e8b552b1111818ba1cf9bac0df10000000000000000000000000000007d3e6f4b1d29ac568058000000d00030001aa1821821800001000a000000c1464ac8a6328006039c1ac884a18304342692b75c86dca2b8d8ea8564100630144349ca762e4348998d7503224e492b4a40c8442ab6ab07198a6d9192092805a4625ee8992aa6152b22545a8ae5280e75a26402cc3ab22a035cc000000000000000000000000000001f479dd2cf4ca49521821820600d5031031300025060860860860860980980860932c88d2201006ad003524b67196691b5994b214a71649a07094022451b489d95cd5ce33272838b22814802b21564071092565a553942712b271452a8ab63199006324cad88b255ca2f5192d2ab7628809ca2222267835ac80000000000000000000000000004a3b65aa17e796be8f3fa4b44671ba8b189808600100313054c0000182182062062000600982681340356449024e28c4d0632521cb6cab20a655d4a75b46a2c684242b24e2d652812db2a59a4a5c4a54cc9918d3890491044e5532c4a068b325e3846222224a5585c216d2a0b6b11271658a100510b1401b824622ca23ab28016000000000000000000000d4c4ad643653663a514cebd627ba8b674ac6ad4d88984a000000310000c04c00501880000000011305434800000934893560d34728ce52510b6a111251404c25107092a40d10dab192a011ca2d4945a322c4ae91955d5a290d451484eb2ae8c489a48915cc938b57192138486c4384c2b538d89348860110dbcce963cf5a40df10000000000036cd6235e4400b19692d328964eeaad96c53b31d79ab4e7df2e8576d59ec21d823ae720eb72800134c01aa0113001f78e034d40144c4134036b1010182000b5cd529ab88a659118898c24a528e404271488a28c4ac90128854301839440001234e69a616dcc0ba5039d446135615d912857333ad02513dd96a09a881af258ec8396714864655251513941ace20409c512946a20269aad9e3d3cc1ae9e5000180305af27573da17dd772f7f22faf56b8d2aed59ebcc5d2ad3159d4a9bc14f439baf3f411bb9fab931d9aecc387a9cfdf9ea6cdf08fbcf2bf4173f2367a5f25664ed70bb92e3cfefb8b67169f43da3c16beff00493e6dd1e77d126bc7edb2e4e251f41f24be4c07402735a5ee8f2fa18e3aa49961a741823b6b4c5a67699d6a73780e953738b26ec7d3c715335c61ebbca7d918f9dd1f41f3f73c3ddd1b0f17bf0fbe3caddd8ce9c3a3e89e2cca7b2e29868f7586cf379fb7df97e514dd4b434e5d11dd9f1ebdbced44e8cdb0c75a2bb2edf9f1cafd19ed8e3aa2bcc211ebf3277d3a2bad777133578bf67e7acecf0fdf720f33d6dbd4b3e69ebfc4fba979997d3e5393cbfa37cb0ae32154903b2b9caebb2b211946e6230d4c31eac94edc9bf3c651b2e01a849aa5d7e469cf6e96cf3bab1eaa7a9c3d5ae1d2b793663d1dacdcd535d8ab992365143d70d9bf8b2cf7dba391337f3b564bcd2ba9df1f4beafe6fbaf3f55c8c1cc3d05dc24bf44c3e46867d9f43c3673de2f1551cbfaa7cafa4d7afd3e26f67dc784ab02c01ce8b467b26fab0c2b9fb7518a579e8d5cc6bd0a28ace84f0d6d756ac75c74d73a6b6e0b63d3c91245e7b3e91f32d3797bba3c3ecb8f611f1171c5fab7c9bb07b1b7c5ccf79f3eaf19f59e1794b0f6dcff236a7b6eb7cc45e44c94dc0b49ae8d753e7edaf6e5baf3d16e431e8af773a5ae3adf3e337b5602e2b563ebe0a66e47d174795cc9a37f183d4757c0d167b7cbe3e061f61e4341f44f37c9c27b1f09bb080354e2131281050812030d6d3c7b164d755e596696bced0a8400201a60d31b8b24d3946996db5db8e9085b0b2ab2171b326fc18f54e23d620495a0021a418289a400440c04c62140626354352800271b81a0900d2608262a601122c09970a719042492173657168445a31351ce6d41db4ca301b88596576a5b14209d6928ce92b8591b2137244e112c5066b5568961192255b75557a126685f4209aa630250638c90020108268430d4c31e959f42631ad8b5cb22d426434c2a82c8d91006d0369927170da92dd3aecc758a064babb66f666d39b3e9aa705be681b681aa18881886900013122d972984d0d0ac4c4c4d0d310c48924c8000c6d03410ae2205e62432c7315a10a0e01193aac922329cd6ab1db354bb09604d24672952275b3170496c2092759146c893828d382492712cbeccf6cd58221a512456596d72894125626818380189495406912112106920675222c69002010589491185a599cd159002c991904e1396d956f3b6e3227755a31db562bb33a41b5aa00a0354c7351188860948443292609b4260a000000c951242182068262a1ab1448ebccd03281a36a6484a129322dd8d54ec6aa49ab1ce581243134849ab191932426267858d295624ae3285017949645211bd99ed94d60c8448add2714961090ac26531ba24538126801a1c24acad4d2449058833a010c4a813463421a189834c54e86652daae5ce0d6c7022d95564ddbab368e7e9cf6d73bda280435600034e569b543162c1129c510d50a48001301a64a9800c10310305215262531b21bf2c648b890ed9aaa7d0cd9e9592aaf09bb26b05385b5a9c1656cebcf56aa2f3b08c12d2a2cb951292c70764c8c48b8045c601172b92ea45728ca41c51645c48c655d84a0aad88e0b2a9963aa4ac5615d76095964044582658464c88c9042562020c47212b00130001803945cb28ca4638f432dcd42352cb6ab73bd524f97bd46c4e90538d836115371024a9a93962c92c06922c6894d1093548611526891254a491a6d62c049b1a1c414d593d0b663d5c58592ebf3f5d1d7e4f3f5db0e9f3e4a2138f6f9baee71e3f4ab94c5c5a6bde665a259f4f1f561ee74f1f2e9bebd79a119c75c5db5cd01a15734224d732b915a90ca251a08a49a112480011293a8b104a20e709c4a70b1453ac6e12231b4285752834231041212486aa4024a48c64a80a0681a70493594e1289ca0d638f7cece75bd1bb3d698dd1e7f4210ba36c15904add91b918e58a9a0131120ae62a699118d9bee79b67b696b8793e77b30f18f77b49af0f1f5bc6b9e13f51d35f087b113c72f75e75ae39eb2b4f3f4fb5b13c2c24a77e8c7462e5eec9a68dfd3cba399d0a79f6d7cae8e4d70a96937e2d78b773797d4dd8ba3cbb9d45f8da95d2a8a3a19ae679f54e9edf29c4b2e5ca301ba9139d325baccd6e75667baa5aa338eb11189052572020608da4b270602101c4251658e364b28a639c6454da2509c082256218670932490a2111b23313080004c0009092c94159639593468ae79d69b30ac6ba54e6d59ef51a72df589828c954531943068006110626d07a3f37e9ef1f49c3a3d0f4f1f1793d7f299efdfe957aef29788f6fe2274f61770355c6fd2726e3bff38f43cbcf5e9f433f7f5cf3f296397ce4969e7f47772ba7c9c7a0e9f2e7bf3758e4f5b97bb2c6a5d3e6dd666d6ddcf39cbe85bcbdd9f7e5e811cb9f4ece774797af36daf572eabac877f90e7585908a0029b8ca6893537646bb11576c0804ee211b92d4ac92544e3621261912a48437190adaec8b5119a9ce8925aa02bae5044e2ac7654cb0ac2b9248109d8d372b02000000001a15462ee5db19352942ccd9ca131c9389eacd767a6ca9eae3ebe43d78ba776985658aa2a691124253811929a454e229262df80b9921cd0e2936641880522cb91089098d29cab664e863d35e0db96e697396bccba796ee7ede6b73df8e3d2cbaf1ecc5ab26e5c5655b18a22af432db1b8d9c2eb7275cd419dbe6a5208c8042072adaca281b8cc9012c6405d5227499072d709477c08ca37001499210c856d762b10a8124e5194aa3622b8ca36218880454d945964d4a183506a0130001a6aab75d92b002719cae49cb394245845c4a706b6dd94cefab2e4ece5e9caf7e1d7a138974c52551b62414866b8d858a516b26a52c54a08464588180c52121126c849083113716d59b703c77dd9ea89769e724e9d18c3468c37dcf475f1acbbb639619d5d7604c4f6f2d31a6fe5bd73d7808ebce096fce365cc54924472a8a9245273962a529426961194449c6c126894e3620482620c4342a6d10dc426292b9d72967149545ab90520013290bae6525294050014c1430002ba8595dd6094a5724e594a2e5938cc938ca1d2b16a5aab96b3395728d7d2e36fe5ea913af3ee934da9baa4d00d22ac454db41a4ae2da42631466950da44121191512410271425144d42b66d8d51bc6d2a6cdb2aad96d9e69cd58eb9ba109d6c2838dc1094ae2b8deee68aa75eb9960ec138834813404d05d9af2e192d621611bd1446c858c704714ec509a4892488158da7280034d4630158b07612d4ac8d89a48084cf6c6772d866a114d828048002cf657a96c872a929034e5728b89ca02cd192c8d6def0308724166bc7767a76a397779fe86337e677a1a346292d83d39e98e325ac21b20d822408912c63276409c510e200d1c1b210b69b8aa2e3bf28946f293834b675b96738b95bae3357570565d582488ab975ca16464a5736465158c9c88bb20111094a6576c59728c46a312d88e5ae3bf1ac045c9171a716d10451c5b48920436a9c99156ce5ab44934576462a528d901a66205909a6845c46c0620627289d7656d59649a72b612834394424e0c59246b234d006034b39d04ba95574dc3a997573f42199f6a9466d4b6629e77041acc84e522c1b4d503223122da04d224e555b622a6ecd715c5adf9209ad70138dccefcd38bd2528e325426138834c210b23645a90c6c938465941c6c26ad23152224ea2d4406a289c881a73b8cd4532e529c2c6e32224e456ec52d448b2249c3b616ab94486958acb1ae4af5d0944265cd632c438c892958c00060042a6caf5264a3126a4ac4e502049c643a2745cb69ea0d289252a4c21b4c9dd4dd9deaec717a5c3dd9a328df529c6458d99e95494ac8b62a6000034c4315290442490692226acaa9bcbcf247453ae35c670d795c5ab857577b3285b196a4e152956c915b59a40e5143945ca22364d4895271ab128929a9224e24eb1114c2508b24a258da2563989889a44a59531265919bb1116425055d4eca2e95d9115d36e74493b2044654250b972004d0c1c09c6ab6a7602712639a00156dd9352a0809dc8050c20180d3094644ec85b9ddfd3e575f8faf1ad5967b494276cf464bf3aaa36c2c18d536e589242262c1828a4106d228c958d38a414ddcd7468cd79d519adf8a0386b94b465b934d53cf041949388324ad4d4d464035625aa332c725396b56d682256323525d2cc8b942c948d950a23d65324b125642b01623222a4ac14a52d737248da31d6584cd42c6035aa3352c71ebcb6569c6e10caa85273602a006d395c250b14924535256d39404537533b95538d92028610000c01a06c64ecaecceeeebf1fb3c7d52cb618f7d2e74ea493ad89cebb61dfcd2f1d73a6c84efcd3d76badb409dd260b11e1bc9e5cf2edf2afbb009da8f33a3cfdd1a7456d50a70d79926b5c609c6e24c051d329734b4456b726dd6492ca5394b4ad374bce76c6c5344a4546e5c2b5ae555761ae494a203817e9e7d937717d336d8a57642c149031a2b52115d5dc36982b5a669d93256c653508c86a9aeea5566baab8ae43b2d223586717780d00d31b4e58c5ab1d73aecb24a52b07295594d845ab121d803002060000301ca3259db0bb3bb7abcbeb70f5572bb3f3f6519afa3a71b0aadbcedafa99a57eef9bd6cf09f1fb31e53c05127d3db5291aeb16c56ea6d4f9dbfbf7c992d5e89e6f0dc5fad72b58f9bebb70749d6aadaf97d1ae16c75c2885d4efcf192b199c5fb5cebcfe9f6b2e7af9e62fa5f9cd4f38abbeef29a2c7583b2b95684e5c099bcca2492ba3560d70947a7dd98f250eff0026b355b6cb9e71a336a3134b3663d59e9597d5353b6b915b0244995ce700424b2dcb7a6a50acba144d7518e535a6141372adc48d5386b11527648913ae212d7924206c60c52c5356244ac9493ce9802cf7d172e2d58a43a01c218260002834926a4b29c6eced77397d2e3eabb3ea38fa70e7beaebc2a64ef2ec76397eab8f5e4f6a79b5c79cfa94675e532f6f8f7d749335d6b141ce5643b4698757a33c7e4bd239eb31e11ba3ce794f71e4facd955b567db184abd79e099be2465df936eeea2e3d2ae967d7995e2a1dbe4b91e8bc7f6c757b5e6fd3f1f6ebe6ebaf8f5a6373de38f61676e5773fb34637cecdd1bfa79bd349cb8eeda345ccf073f6f9bb7988fa19ea78fc9ecbcbf4e35d13af78e9462f3d65384c52884dc02d8112294596959516925d6536cd8d134d35371056421385ccafaac9d511275e788ebf324d395b52948b44471b95642c56d4a54a5115175172d4a36363006a26c8b0000018a4a44efa2ec6f7eaa3a7e7f752b6cb8fa38f0e9e6e9c30eee6eadf28fb6f11eab2ea64ab9a9e832c71e37572abbb5e98494dd638b7e2bc6cea71fad73ddd38704f374b7f276eb36d3d4a263c9f23d070afb68aedaf56baadab5e65125ae4fe93c2f5fcaf86abd9e39adb54b818bbf9d0ec6dc4f0df43f9ef6e3a3d3795f51cfd1a7453abc7ed9d3dda79f3c4f7c98e553d32efc57731f7bdbe6c70cf2b8f4f7e48f3d59cde455b9da5e7f72eaf27dcf3bd39e68b3b79f72b23cfd088d765ca977372832c2b6ad26ca95a1091296bbaab1a22935370734e0e36029aa6467699233d39728cbb7ca6d4a56d39520455d95ea592529a6d3c9265473df4eb2262390d5360860860868001b4c9dd55d8debf43e73bbe6f7e85ceddc3d3a70743b13cdf3f9fa697a7cfcfdf5eb59c29e6e35d0c5e832ef3c85ededaf234faeab53c8737dcf1a6fc8f6d64b8f49c4ed5bcf7e5fdce5db79acb6797cef6702daf5eca216d5ae7553a2ae9e6539b63e85d3cafcfabd73a8a859cdf519d78fa7dbf3f7383e0fd878eefca7ec7c77d239eeadecf9feabad84dc7373bb15eb59f4695ac72aeb6ced78b575ecde5f97eff366b9f57a2f3dd79c3240b67cfbb2ef946d776b3329963a592d15c519ba2ab04e65b09032e718d96a8a4b20d2b20964eb26a4e2d5c5ab5d8a78ed539274908979cd4bb7ca249cb2025516ac494d2524e69b14a80b2bae71d662c904872a1803403421821889813b69b26f47638de93cfecb7ad45be0ef6d909f7f365ade8f473ebe7d593af18d95cf3bdb379fa72b31dbccd5d2b3bb6ca72425e15bdcc5c7a723d1735f3dfa4862973df2f933874f528590b6961785709437c6e9d5a98fa0d73f2fc35e96af3fa36cdebfcbf6f969f1a9c96f2fcef4307b3c967d13e7ff0050f377cd7d7778fbc3564dfac5b4cb3eb9eccd42d1e8c36f4e9b32f1f759c7751a77393e93972f173558fae21547d6eb971e5ebe5cfa78bea4b9baccebceb53557970d975555bac7462aee7df33ba1ae5069128baa926c131a1a72c9b9ceae4cc7a60e42c098729a7dbe449a9289c6522d591babb06d4a57194655116a406ae54938602b63953010c10310149823ba9ba6aff45e7fbfe6f5f72ad6797a470677e9e1bfb51977f3e6be658efe56c2daa51da8e3eff2f6f763cfec13b2c671adead39b81d7b38755cce9e5cef265eaa5f395fa3e2cf4d145f1d73cd5dd56f8ae97376b3efe986ee3795e7fd061dd2abb9b2987579ddc86425e8f2743e99e03e8be3ed0b9ae08a9d52bc3bb35e99217e5dee7af2c779bf91b4d3ce4ba98b73d2f9cd9e7f37353647bf0eefb3e7f5fcdd4c7bb066e3e5f7f85d1c2cbdcc1d33c7cbd2e7f5f3ae8e4e94de6d3cfdd35667be0cd4adac88a54a4e53517626a963594a067d17919e7ab639b430e331f7f8d269ca90ac149126395c93948ca254d1ac8982630025934d4190861119609a04c1d95d92dfdee177387abbf9658786f4e5bb93df8fbc9552ede79c285cf7b6b35cc510793b5e379d25a7a3ea65e9538df513a4ae590945b410cdb34dc988a94a2aa753ae6f88fa6792cf4f35d55d1e7db6def97974393cba7a6764b046b2722c3b79a3ddbe78deaf57e77b7e4ebba595f39b29a2bbaea510d5d58795e93936d38368d79be77a5c3d671a5aa3659cfbf3a55e8389ecd9eacfcdfaae3a9f3f5f0a5e872dd9bb878fe8bcfea62c3d1c5d79e9a166b2beaf2faec46b509ab6b57545ce32c5a6b2073a44baa9da2d13564eab6749c939d018715a977f8b2052a4cb236c272837000a45c6a00ee44c131ca98c724e5060936446111951608ac84e5d1d4e4efe5e8f519fa1c5e1bcd0cdd6efcbd195e5667170e1e8eb5fcf7be17f36fc5d2717663f41d33b2eaa5d33a6b2896ecd5b48b9c086dcbd0ca688cccd3060c5cee9135e47a564787a2fe1f6f9935c1c1d4cbdb9e7b1e1d63bd6d71e76ee4efa5aeb4f9f673edd8db96dc73a77f3e9e92cf55e5fd575e4537ad67c6eabbcd73f476f2732a9abb0d39ba66cae32d63d17accbd6f3eb16b71cde6e5e8d5ab2e357ab7179bf45c2b39f8f467e98a2ab2be9c2ee9e1bb3d088d2332b5b541cb39536b765b9a79efaabb258f5e695d14aec936a0e511910e4493eff15c5a944dd9269e68d49442126aa0d3b960e54c62639642164294252421ab129045328945c5da72eee7dbd479fe9f2b975a3d6799f5bd7898ece773e9b7662e8e3787a14bedc27cee879fb33fa1e374ba62fb72434eac7048d51a11a239f661aef85932557245646542712c104b9dd1e34d61bbb59b9f5f3fcdf530d3c4f6fd2d9d3979c7e8b3472b455d5e1d30abf2f495cf35ba8a0911f69e43db24c74dc51e1fded58e9f248aaba5b54452fcfd14fa5d544fcbd6caf9897b91ba2ce2cd673aeb165dfc7e939f47a6c7a9cde5fb8f3172ab8c37ce5115ccc4d66326872b33da068967d259179f45846ccf4aa528d894d9593138724fbfc3516584d3946886d35516584440d30639418036263964372c49222a6ac8a9222a4ac4d48bb5e2bf1d3d073acab97a3a5dcc9a7af9a3c1eff2b3ad1d2e2f6b8f7ae1653d784b85d4e26f3bb572ba9d3103742b03b73c2b2a866ecf43877c929433b3ae755c10b68273ae4b38c9592e2f585ae560889531351919e8df35e7c2ccd9dc33db5564a6dc1a6a9d16c4fd878eeea7a15195c9c8eb878af29f5be6ce9f2c5ebd5792d1dccabecb1f469f3f5e3752aaadec554e5ca79e31d28aedbb79f3957ade5358b9f9f45ce12dafaf994cb4adca53516ac9d2cbcbf9fd0ad5919d864e6a0d8a0912122402f0d38fa3f3e992b1a0946a4080232889a29b4e18dca49592d526c4294b36dcb056448128d91538d894a362044edcf6cd7522b673ebe81c0d72941a9793dfe46fe3e8d5ceeb7175cebe1f5f276e5b274ece99a9eb89861a73e2d5d3abd3e646aa6eb324b0d1a7a7b134745f08aad8b96710b2a9ca4a488254a245aeb996d70ccb5e69519dc73c69d218a6e96be7ec2dddc347d26daa59ccc8bb2324cc56c2e9513761293d66b7549542fcf9b933f52f5f21a7d33ae073bd873b37e537f7b978f564a77f377e78dea7bcd603529475e3d16c93e7f462d16d88268004a6922d163025e220f47c0249898400e84208b5434e1b5251844adaf467453a2acdaa4edb19296755c6655519ab2319c6c8a6ac8a92b14e161afd179aebf2f476e246f19109b5666bb3e3a7673592c3c9476d5eae36e8af5eb39d6c866e7ba5dcc2737cfd6299e7ccb2ea733a275a509580d4563af36c9c5595474d4590ae6b593919ddc4ab9bd4e32cb25f8d72d70a348d13aeacd98349679ced73ae7e932f9c7d0b96fb8737633a082d66a7c3d59deeba8e159eaa3c2e8eb33ab4e5ceaed1cd82ecd386c6763cd66f36e37c4e5be4e2e374f97b2bc97d3d7cf191eef59f3dd5ed1cee43a16cbe3f8bf4ee06bd5e44b14fa3162134329b6a86d6201c207e8fce8d35001a412838809d0c21c94a56352cf45376752719e6c89525869a4aa365642335508ca1acc54a3628ce3646702b575b87d1e7d7d2d5cddd95b6551974e15c3d3d5f4bcef6b16ae17a0e7695dd9ba3db853afa57e6536a824bcff5b856eccb3cf2d7e9bc57d0316d717bc4e2a32baecaa3456edd4cd1d19a55a2bba146512b9c2c31e0d7926f315d5a578364ab893d18ac8ede64aacbe98a55d6e7f2cfae4fcafa8e1d25571a0bdac5855bafd178e8dcfa0cfd5ae5e1dbd2cf34b561d69d5a33ecd72ad63eb1c7f99fb9f1177a3aab679fd98ada35eb8f6fabe7ba1796bb73686ac71b10d34bb8f23c9f63e367d7403d11522e41a518e5430f3ec7e9fce2001348c22ae2d5834c6d3964e3295b096db2bb31a9dd5396bd78fac6dc3d0e773ed96ababe9c2b8cebb6109c6e62a51d48a946c8a71b1e8cd397b367336f3f439f2a3ae7d4e5ca1acf5fd1f93f43cfaeb8c3a58b5f4ea9f6f34a31823a1e7968e66aa2a5c4b28e5d3bde9f2ebe9ced4a94b20a997614d8591a0abe1302c4040a624e8ccb760d754d4795d2c954f37ad1d39f5dd9ab9f2c56eb3054dac965dd69ae17433e33dcf63e7bf42e7b9472f0f3ae9f9aef67b6bf49e1fd7c68adc63174b8fc0d4fa3537d9337c633b8e67cbbd67067a3bfa73eaf1faf93dae2fa2edcbca74fab9b7cf9cb87b7af1f41dbf9dd527d4a7e77d166e7f07eefc1e7dc26afb49215b09a4c1418bc04d7a7f3402188101611686e321b5295ca3295b8ce59d909e7575328c5ddfe4fa5c6aff37ef3c4f3bcfaaea7be2aae7014651a51942c51947598a71b09d723574b95bb9f7c2ba79359a699c37cf577bcdfa4e3e8f43a6da75e673ae564692894caf28b9857cfa537e5e969ec6caa7be450ea974517572dd5e0af97a39f6d4b4f47bfcafa5d71b2253ac3c75f32dbf479ff004ca533c79b6c32eaa51aea21976f1ab911a9f4e73d557a29ad3a679b9eb859b75da9edfaf567c32f92e45b75d7d35dfc3d1ce8746166594f06a6fb7360b3d5f5b2d8e5d3cabca2794ebf27d04f64fa1d2bbcd9e3f574516434648eb7cce47ab7bc7038fb79dd78e9f79e43d74ce2f25af993d5a1ab73f460e49d0001a164225f3e07abf3421008b012418a9b5295ca3295b5294b2b9e6cedaa534e75694e87a2e2fa2e5d2ff2bedfcae71c2a6fcfde549c6551946944561094359516ac4d1659af15d9df7799a6be7e8e5a677f23fa2f8cfa1634e98d5336caa999b1dbca5b38d5579d68aaab96cf4fb74eb329c64ce48d739abea98479ddac3cbbf0e8d19ed7d4e361de3e8bcae9bbcbcce4f434f494f574e2e778f93b326b9193bf86b06db78e9d1e22c1a94caaddacf4ba3cde8e37b39dd8866e4cb74ebab5f336c78ef47c6e9cdf62ccd5f9fd1a634c2ce8e6c17d9d2c496b3dbe971bb77951f2bf47e57ae75f53157cfb6bd1c7bf7c3d574fce767cdebcd406e6ae9f3ab8df9b56dcbcdf0abc5e8e1674724f3eddaa1673fa314caa8955785b2cd616158d71817a3e089aa4090116026394652b9272b612bb2bb33a6d359eccdbb1aed75f85d7e7adb9eedce3f36aba7c9eb611956ae2d58a2d5461386b2a328d8815929d5336ece774397a390fabec7a70e7f6adc7267b6a966ce55706a3c3a65a97d51d7351d3675b3d3bd65365e3638c0e75d8f5b5a6338c6fe4f5334bc1a3a38a74c1cad79b53dbf4b87d473e953804e8e0b7919d1c1daf5735529ea435ec9cbcac1dbb93cdececa326f9d52bb6ab8cab4652d555e72b91ea7c569ec67874f9bd366ec5cf3afc5874359a2e9f7f59865e3795df2ab663d5b9d7e5f472f3b08d7dbdcebb8e0f37abbd96ee84bc2bbb5cfb25e472e7ede78e8aa7b96aaccf4e94f269e5f413cf26af75a7459af95e35998d70c69c7afcf111b1c48d925168da6b29272b6a52b689656573cd73aed9abb763e8f2efade7af1bebd7cb3a73e879beb7335ce84e3acc095763446c4a4ac8a946c5171d65ca122fdf87772edecb779af4525b9eac5ae738f1f836f5b8d0e86a73e4992e8f3fd2e3acfb9645876576b33cbaf9466d7975dd6dae71cb42af41c4ae5b34f03dcdd9eb3e6edf1e5ec753cfda9dec9569c6abf3f0dba73bab93a2938bae59dd5c09acf03a1462d85b6c025cbdd517513c43e3f528d4e577fcd77f1d37d992ac6f5613a35d2e9ac939fcfb1d72f472eb570b79f6d38eea2e29f57c7e9f3e9aeae3f6b1d29df54a5d5e6a9d3d78ae57aaf2bbca85da1613aac9a4a102ca6abae6cbb1cb3df6b59b1ea999cdf931a71ebe349c6c438d0269269c4a5194d36a52b02594e139a76d5a33ad3d2c5afcfe9d55516e379abd54ef34d17c378c50b6ae9c229ad66235628b8d89356462d6b28689e8cb397afddf25ab977d1c84baf9c029b884e74d99d6cf71caebcb6109b3375d859c3ebf9e5d5bb0ea5d909aca3bf06c383a69af4ab97d0e6d6be973366751e4753b49cbc1ebbc6174b6625d12ad8e55462c2ac15a19cd3a3bb3e73a7572c3a11c882a8ec2859bb6b6fb5a36e730a1e7cea9d17c25a2ad39cf92edc9d6ed9753c79d3d7cddbd38f73b5caf41e5f6e3cdd8cd9b87cde9cbdfceb6658f5e3d1bb97ddc74f3d65986749199eb9cedaee96545b62d17c252d79e75dcc898d628ca1bf3882945ab0698e51944a5194d37172c80965657396cd346ce7db5c9d3c7b572adeb33bb2b96f8422d5793563ebc14650df2110b9135628b5a9113b04c094665b767d1cfb2c9d2c1ac400d6251406dc5dd97d75373ca8d39606db68228e6e9c9abaf451aa1d99652e9b79b612c1d1e2d5bcddf9ab677795ecb28db9ae4e1f27a5c39baecc51add0c732746c665967cb51df884dcb9d59d2af7fb1cebc7eaf576e2f9acfea4af3de92db999d7357256b36752b2879d154f3b5f39afafc8edc8a6cab788df4db46acd1976cf97a134928d3a1ccbbadc7df9d6cf3becfcbf3ebceaf7e6de079a766d52cd9ddd4d95591b62d2824599e328eb99194488cb134c6d3894a3256e329a6e329653aeccdd3bb26ee1e9d3cbddcb8b945ea3625941569666be8d62316b7ce29c75922e361171b2235632224e754d6fb69dbcfb6acda78cb06974e1269cd3ee713b59d75bafe1bd75cdbcbeb55242ee3d8bbe8bf29768e7681ca9856a8460bd1f37e9fcb9af45deaa2c8929199f9b9b671fd4701bf2b0bacdc8d1d8c92f3b1752367329eb5166096e8141d3eb4bdbf4709cc2a2e52d0ed8e6dd0aecb1c63cd974ac5ab1b33a16ce06cf276f4381def39d79b98f7ceda932d83910aee6553b6548530d7974cbd9c72d7cba79379baba6135e72bb4aecb68b194d76d57322c0c89bb98c651b220ac0024e328938b5938b964d39656576e77bb7e2e8f9fd58f0ce1be522122c558ac575579efcf70a2e3be6448d89376415caa88e88dcd04e08dc555da30cf3aede1a3a38efcd90f7c13b89ad3d1c174d54155cfa8d9e13b5277b3ca650f54ce3d98acad6b34d6fbf9ddf89707b9d04d5a2354595ca30b93d2f3b9e9d0f2d2bb4c9d3e57597439db1cb9f5207117a089c93bc263f4fe6b875f458fccbd25cfa98c6524064d428d1933a960b754b80d95cb1aaff0022b8aeab4ef2b85e9bcd6b2272e9ce229129464926a630628b4597e3d0bd1ef79debf3df9633e7b75e594ae69d799d96974a6f358b3336959735cebb6aa84ebb95169189d3719127172c9c5c49a7353baabf1d3a364f91cbb094ba728c92272adcaeca52df93466b08b8ef928858e716ae2d08158a32572a3644a0659674b2ebe7db2daeb45ab2c8e9c74e45aaab29b95591b37767cdd47a433425d9bf34d14b48af765cb97a5dbc9eb228e5b73a9591a8a7174f82be735fa7f1da6ecd8ba8bd2dfe77a19bd59d2f2bede76cb2dcb8ba55cbe3b9b5c83afc3dceff005fcedd97bdbbc0f5a4f498b8d0ceba50ae39d697cfe20b242fde65b2ad7cf79381d1e776e2990e987642449c2c494e122522b5288c12edf8b62dbd6e36cc6bcfcac5509530b35599e135a2ca5ad688dc585a4d609465ae70ae70b22058c2e8a89c09022528c95ca2e5b3663dfcbbece3eec11669c4f59d34915938c524a2ac93858550943591c656341280ac693449ab2437359cbb4128d56e776d56d79d42ca77eb9ebcb7672354a3691e9f3a74edf6343c6781e6fe8f86cf015face46f3caecf37659e8b9f5558df73d0e6cdcf5d679735ccf3d75db6579fcf591e6cb674c5af9fbe5d7b31d79d7737799d52f7f996e294edf1fab356f37bfc04ee64bba373e66ea7367aebeef97e9276ebcaa4d151c2c6b0e495dd11d06ae5a942df33ac56d1e9e118825aa51a77576156de7ec2345d8914a16a6d77c26aeb96fc6fcc4435612065d56140a08edab52d24831345e718ca3493564f466b25820b18a50dc5ac9a72ddd0c1d1e5e9c158b7c66904844b28c4b1ca0d1348b29baa20e26b3301534ac6211a1939ab31d3773ba7825a2507ac6850967a1bb0f412354abd660935eb712dab3bf75a381decc9e6d35e6b35d72f0f97ebe9d381dbbebcd9f3de595d9839fbcf772f9ba3a73e9d57f56bccebdd9936c2eeb65cce8caa97166ec25e15bab936757b9e17b59e9d2df973677af571fa92be274769c9cfad637575b95cfd67b7c8b2dcdcfa2f9e2c26bcf5cd796e8fafcb07135137134c24c84e200e4979777b974f370ed72e8aa376f12e83c58e9cfaadaf5111763698eb9c435d308081739986b3142b00000006124e06259ca1396fd99d73f4e59d6fa79e4c52ce2880458c1ac46872ae4421696446090ac6444728b2eb6a9e3af473c9e35cd61d793957396cea73f5cb5533aac838d8a39d3372f59e3af67dd4f95dbc5d544f04bb72db965b31ae64d67860b77978b5f3b79a6537be54f7f8703dff003f17a1e7ae55d4ccbf4e552eacd6dcbcfe677ef3cf63ee726acebf99e963af41e3c3cfa76de3d39d315d8d59c8e8f137cfbd4d91e7a22713595cdb21ebf2c6f855a8d5a228a2af8d617406929d7d9c6b742dc7e5fa072fa674e3cee9766abcfcce7847b739a5a25aeadd9160e32d60aa71b96d48808295285ca5211292a4c0018038600edaeecef5e1e87333d589ef8b526a2e8f3256023710945a0685716aa446c2119c11215cb9d732dba8bf1d67d3e5f6b9f4f3d7d76f4e58e70773aef8a5aebb29b174f95a26e31ae6904dd3edf1a897e88789f439e9d1c57d3961e377301cddd557667aa51ebc549028c9595fa0e1d527d0797cff0043cf7875e5cd5b5d99b2be74cd5e1d6a5e3c35666f54b35fcfb68b724f1bdcb2bc5cb3e47a4edc6657c5e7aea79f9bf479f3b9c3a604a48ad502eaaf815bb0486ccde939f5a3af9aaf27a68cf52ebd77df9f6ce57f9fd7e6fa72b2b81e8f3d9a71e9ceafcc5134cacdf293895375c86216a8b6c83424c488ca27022400a51912d346dc77973f56512b0d7352096b62b196d24a23126914a3259212965560576d6406ae094664acae79e967678bd4e7db994dd4ef834acb3a19a55528b8114d592d19efc75cfbe8a9ba2ecf6eb91af1b5f453e2ede7dea85f999bb0dd8f5cc4d6f92716205609855d5e7551ee5791f478d4b7146770afa1491ae376758a3b0cef34b4d99d64e85d388703a5856155f876c45d9fb79ed2b9b22688a93b2ecf6d45d1956595c674fb1cd972e9d4cd8e8c77d9ab9bd6b76db6f98c31c147d3e4694ec9cea73444694b1eb0db26902264c9ac76512d73b13628c909a68818371524a64fa38ba1c7d5caa83af9cb2b984a24b22025954a548714837124e22ce321aaeeaec65d738cd56a4b5cd4e2cb251967a4f7e1d9cfb47075399ae31d55ad66ca914e033a1cce8f3a6ae2129d35513d18f47256acdd7c8ee8df12d59972edb735659453a7375e0991b89496d9d702b2579e672764512299b82763abe46dcebd6d5cc963a7a3b3ccedc5e85367433be7dfaa98aeccf88ecf0f5e2cf5cda6fe9b5e36b9af4f922493298964c824a28b24a72236a92d118c472806ef4397adc3d1cbf3b666ebc6c837acd7642764650076ad99df3ade8519d4b1f4f346459afebcae224d67aeeaf788595366f55590302328cc719257385b3576aace5e9e701d7cc37296a94e3511c124810691351090a4a31b5558866642c9aae338dca6165813ced6dc7a71d76f27a7cf7343a7a60718d8c883b216e7751b7017df91e7ae8ae333a1cbb629a689296355db2b26591be566ce74648ebc76d599dd82a88dcc6dacb2c8c82b564504e328988a71bd60eea26a91bb8e87a5e6fa2f37b3a1ccea79fe4f3ef54fbe3937745d99b5c6ec6ab8e8b65e7f3fbaf59f3d66ba7af3586ea6c49ab1f431fa8e7d6dc3ab072ebc08cf7f7f37397aae9f2df87d9eb30e7bf98e8abf5633973b2bb167b7af0ab2f6399be57d9d4e7e7759334c7070d7288d584a217945b05b0b160c617d5a31d3562e871b3d403a79cb2519b6d39650b2b210b1dc56e4aaca3766ceaabeb7acc3adcffb259e057d044f032f6f69e078ff005af989e78416d955d8e8afc9a33d3a3ceebf159840875e328a4128db352b2a26accd64514b6e2b55c2cd94ec9e3b5745d8f7cb67538faf3d7aefddd1d3cbf26a7ea7559e3f67b9d27c9791e87ced26451b051c42600a51b22294413549492138eecefb9d4c3bbc5edd3e5fa7cadf2addc6f2aea6f216252dee8b62e9d3696717a7c2d4ae1757d715962b9e9687472edb6ea6ce7be9ba23c3d7a72e08eb473afc1dfcf3f4993b39caf3bea38f9d7977d7c1dfcf1a5e3df2ede5c9b5a89317951947a79c18252421a2db72ca2f719acf453a79f7b795d1e788db8758d71aaf9acd7d7b66965f49e91af99f7fd2cb7e7f9c29d63408590dc69f79c9d965be07ddd478af770acdbf33fa1527cf51f405f077fd02c97e6f77d0279d78ce37d36aaf9a1f4be0ef979023295dabe9135f343ea2acf984bbfe765b2032738fbccdf218be9f06be5d0f49e6f7caceb73bdacd748ad5ce98d10b3660ba47cc23f49f9ccb03e81b2cf9cdbf4533d3e6757d3ebb8f99bfa72b3e64fddf84146701b9f7b1e8f3ebd0bcf6f3fd2c9d170eb68c0bcfefa896dd672d1a29be750b26de6d40ee0c8be10aeccf9afa3a792b8f4ac9df9075b35983a1cfbb5e6bb54df2f76ce4eee3468557a472e27ab171efa28cb4e3a6cab369b8c75db474e3c2afd264efe6c0f24f78d6564d73e13875e081a21a01824e23ba823a3bb91d9e5e9c35d51e9cba35e7bf1d31b8adf1b36f36737eebd470fb5ac68c5a7cd9e1e1bb073ee9c63be32fab7cfbea372ae8cec8d3756516cec23e7bd278397c9fd9be65f50088ac719c4ae530afc07d0fe3e60b23d1c6edfaefce3e87638c56b3e4fc07d3fe693555bd6c79bdafa3e4d5ac0d42be59c7974a5f7fd955d96c08938a8174f06a38bf35f59cc97e953ab459085a14db39151391e23c0fa1f3c45346fed61d9e7fb4e0f14df3bb7c3eeefe5d82397d97d2e7f4e639f93453af9f73167eb8008622646a9c57d3d3e4f4243e7f52187a1cbdf928db8ba9bf2e90387d8a78dd1e7f6f9167b2f25ea794d1c7d9cbe5ed8f63b77ebcde5ae9d19dc73e8a3584e9ab588f27bf97af2e481db8d29abcc14a10d534024d0c6e1f5399ab3d73592cfac5e4d63a513adef9464baa7d3e5666b1790f6bf31c75dfc7ee61e1ebe4573abd1e3f65edfcff00775ceecda7c896dff3af419d7d1d8b59b3e53f4bf904bddf47f3d4bf5ddfcceadcae6757e7d9d7721e2e9c75f5fe01be9c6eb953cf7eff00d5f37a5d39d52842b27cd3e9df289757b3f37f48ceaf8b5bc3e07a0f0b2f8ff53e57e8535e96b25ac64f3cbc0cbf43effcefea566296981f32d3c6973ededfaff2ff00a65c74884b78cbc8e4f99e7dfdc2f9d477c6ca5c6c0574bdcb11e6fbc72fb3c1df9abeff0007d05e0d4a3c7ebcb6e257c392caefd72b00c7d38d2477f3acba8bf3ea0233b609e7dbd7e5e86ce5f5abe3f4b9bd7e547b7caeab64a2f9fbf975c2eedf156dcfeb78f5a232b78fafb690e1e3eee7d9d73b68166d05f1d6299146b3619cd679083d1e4728cd44d4241624c24c9416434cde48ce761bb9f3ceeabe0ec7eb7ca7d0cede5dd1d73e7fce7d878dc77e8cb9da38f7e5296fefe4fa76872d623f37fa5fc64abdc786fa7cbd5159670fe6decbc54d4b464f4a9f4b68b0f947d2be61cfb38b9f3f4722faf475f248afbe7d14556f1752ee33fcdbe9dc895f629b51ca4547e61f4df8d6774fd77e6bf53b98c6659f3af37d2c19e9ed7dcf9fec6b9ddc3ec78e97c8b52e7db4fd57e7ff0047df2ae36e0b9f03c6e8f378fb3226bb791271b0df83b38f46d4d79fed4b9b6f3ba7cfb7b9cce8e7b0c59f6d34c16fe3cb6e2dd9f5c494f3eb7dcb6af378b9597467f47b0a2fc1bc51d2e6f535e66e32c7bf9f8ec876f89b3766d3cbea14dd88e7db4beff1aef5be47d679bd75f7736fe7d659b470d8f37cfe9717d5e6f52727b1c7d094a119f3e8a77ce9266b3c503d1e494a32945244071b09466126a596dc53ceeea6d53a515d95ef884525bf5bf997d589a92b3c3796ebf2f9fa6b90ae2bf5de43e93ae5dfb2acf655f29f71e26587d9be5df4fb2c9903e5fc4b212afa0780faf274470af37e37b7c5e1e98495b9efcb751dbc51fa07cfbeb9acee8a76325023654cb2aaab355f4cce17cd3d9f8ecefd5fbdf3de8358399d2f3135e1a6bbfcbd7f4194a3dbc51f99fd2fe439dd6c58d7b9f59ceea74e6bccfa7f0d35e633ebcbcbd18548ede580161e8b89dfe3f458a5cbe9f1f2dd0f47c3dfd0cba387d6216e69acf14ba7c8d7aa9bb9fd735e4d38ebd48e0d5c38f2587a3d0592f61cfc3f39ddd3e675e8854eb7820b476f91d19870fb672babc7df8a92ea3afccd5ebbc3fa7e1dfbe55b38f6b3cef7fcbdbcce3f439bebf1dfeb3cc7a9e3e9ab26bcfcfa67aeea77cab206f1c869fa3c9294652b40b18ce29169d9738599d434e7e967a18efcb9eaab9ae9e7e872f4dc76fd9f03d36b19ee382781bb2eac7618b1d2bfac792f5dbe29eb5be7cd8f5a662d1a2b2ae375fc71e2dc49757d97e6bf4db1c5f30f9c983a3c3d51b49f3f470e21e8f05ff62f9c7d1759aefcdce4d7a3cdfa21c27948747c6fb65a2f04f96f1a5d39afa55f28dcd98b4a335f749675cd59c8f9b7b1f1dcfb46e877a3e8ac7d789f29fa57cb39f5c10ba8a4a659429c6e3a7d3c7b3cff006e2ac8e7d000c886aa4a4b57375e2e9f2fa96e1ddcfe80353bb0200d926be8e47e5f371f387afba09688180d4dd7c9e860ebf29d162e9e2afdaf8cd5cf5ef2ff00196f9fd7975d98f79e660d19fd5e2d3ec3cdfa3f37ba9ad68e7d7166df937c7281d38f1c47a3cb269ac809484e245b2c7384a25ab2dd8e90a255eb2e75eab2fc77d935f5192af5ceef0decbe6661bb3d99dedd5cfe872f57a5f47cceaf5f2ecaa8e66b1ddbbc2f48f44a5029f9b7d47e2c5604bef3d5f3f7d97799f47e2a6bcbefc9a38fa34db5ddc7d5e69db47abc1eefd461e8eb9d5e57d4f842bf7df2cfaa4b678eecfced7d8fade3762e5f1fa7e48f1beb7c9fd126bd2c651b851e5f3e6bd3d7c6efd955a493e71c5b6ae3eb5edfc37d4f7cbaad1d38f9af09e87cc72f43c7a29b019652ac2e3b96718e3f53b271a4df5973ba19eb21bcf74f262df96667ea6fc5a44f8fd80cd8f5e6ea98374eaeea279d6a7bf97c78661aefe91596ce79dd955d0d0bcbcee5dfe1593b89be7d7655bf38d3b1b80ba2354a2dd3814df63779a31d7d4e1e67479ef2961ac70c0f4f8dca3256d39406a9b9456c2c77556e7755775b663642e27e97ce7bf3d2d36d7660f96fd0be7ab292db9e95df2d18e9f48b216f4f343e79f42f900bd7f90fa2cdf6dd86b1c8f96fb6f132ad147a23e928761f2efa27cc31d6bdb8b572edaefcb3e5e9c79f6eeefe6fa0ab21dbc8fe53f49f96e3ac3e8ff3ab65950bb0bf470ab7c67f34fa2fc9a6e3f5ef9a7d4d2139d773e0381d0c9c7dbea7db707b7d7cb3e5f47cba78caeea387b2efaf7ce7e8ddbcac5975cfe6f92ea3cff43a3daec777bf87c570bea5f334f3804d8cb26a32999e875b07439fbc033ece664b6beff0977795d6c7b8039fd0e7639d7dfe1f436d5672faae50b337a3ce8473c640b5eab5bea73f0f193874f54aea6535d3d3c5d5c7e7cb89d1c7d671a128fb3c12538227174dc58c8c9470637124d46533bccd1d393945927172da04d16424d4051b9b34e3d39d5128963af4d22fa8fcdbeb9719ad8e7b3caf94e8e1ceddaeacf4afd4797fa0eb9f71599ae33fcbfda78b53eb7f35fa616599ae4f9e702eaa6a3ef3c37d4cea5328eb3e7bc576fcee3b5b6e7b31d2fdb8f771f566f51e77db75e1d3a94bb78fcef88f43cae5e9c668a26a3eafcb7d175cf65c43a70e4fcf3d6f93c77f49ee783dfd72963dbe6cf20a7a78fbfe8b633bfce3c1fbbf99e3be7a7555cbd7ebbd672fa5dfe74bce7a1f0ad799b0ddc7d9f4db3ce2ebe3f47f1cf65e1d60494b1d355d9e93a6509be86aa2fe5f508595b7cd35cb7f2abd95d98fa6e9b72af3d4b476f91d04d72faeea7c9be4ead94db3ab0a9d74773cf74b97cec500e9f48cdab0df31977733a7ceea68e4eacb265e8e2eb8821ef9a684602c5886444620620a9356394642921673aedce99326eaaedaae2e9a735a316adcbcd8c19d9f7de5bd46b8c1dde7d7c56cbe3cbd786a9c6e17d4fe7df47df2b4cf6eb9fcfb85aa8cf4f43ed391dbb8593779a3c40d63addf58f9f7bcd62c29cf73f3cc85b8ef1d52bf9767a29a33dba1efbc57b0ede4b1d19ba70f09af14fcff004eaac93367d2fc1fbbebe39448ef8fcf7953dfcbd9f45beb3af8e7e3bd6f81e7eac9e8f93eaf9fa7ac417a7e666f9dfacf1fc7d96e9c5e833dfda4ab3d1f32df99fd03e75cbd155aede5eda736cc7714c66f5ca0af8a572b9b79d5d28df20e7f55d766371d0f1d97c9a80cfd132ea85e3cdd71d3af3c84f3edcdcadf97b7cbe9dd0397d0973fa3c3df9fabaf8dd4cf9d819fab5d0ebdfcc7cedd8b7e3a6dae9e9ca73874a6f24adbe74c15e8a75c89c6c6a10baa4826ae1003222440a6d31964658d95cd6db289e7a145b1b9b5a25d78864e06a3dc6ca2cd73bf2c2673adb6735cff001debbc9e7a7a3f57c6d3ae7b6b8e1b3c8e3efe2e7e8f7373874f35be2fd87cf73d31c6f8e7a7acf47cdd9d3859c2ecf93978562972f55fa71ebc76ab06fa359f51e8b99b3b78afe3753cecd79ab3651c3e8531e85276fd372ba1e8f9d6f2fa1c35f27e879be9b97abb254fb782af2ddae4797e867f67e7bd16f16159dfc5e4b89d2cfc3ea67f59c1f5d79ef2a3bfcee7790f4dc0f37d18faff002dedf7cf33d15f4f2f81c6d72f6c827356d868e7d70db64ee813cfae38f4e7d78e8ba8d9ae7a4473fa0d05802146c4cf367aabdf8b409e7db0e177706fc183bf8fa0da1ae7efc31cf775f8b0c17e6e9c223b358b7567b39f77ab9fa9b866be8d61db5db34a9ba8b98464b5c62a4843083458da9adb09d72c651924a51736af2fcef3c75e6489be99acfd5e7f52cf5d0e44ee3ab1c105dd2e59673f9b38e3b7bc9f0e7be3daf2bbf839dece871fad9ebdf9f0a1d3cfd6f03dce3e3b3b25a73d3da1c33af97b7e0fd079fcf6cd2d2b9f77a6bd38ddd83a6e63bc6197a3c7b381d1c3cbb155e79fd0b97bacddefcb9f3f57836f175e0e7d73fa4e4686ba473976f3ac1bace5e8b36f35ef8f46ac14dbc7d3a9f93dd3ee707775f26f30bebc79fcbec55e3f73eff0df7e1dbc1933ea722bd93e5ece7dda5192e9856e56ce943ba1374e6d3474e19b4d2ae7a064967d1a4c81accf35b6baa9b8d3662db39b35d39ed9f36bcfaf26b5253aaa3365e8ab4e6b77f3eaaafaf59aac45cdb2829b52addccc5368b22f3d234db5eb9c53579a85815932cac009c5ad901cb1900ecaec9abdd73ceea8b95ce9bf0eac6e990a6a76d24d69aa11a84631d739db52b0957297bfd9f29a758f4479c8194a4c76968cba0a6dcd3b993a59344659ca92b5598edceb5baae9735d89db74b3a3640a5753ae32ee960b73ad308c2990aab4f6fce6dd73f48700df0eb709e5c7a2f8d267a6855116cab996c5195d074c5aeb855aaa2c84aa2e6f21735915a5cbdd86ec5beb2a8ae99e7e98b144ab2b51493ad96dd96d95556c12be861e846ca486730cd7e5dc96de2752f38f2fb1cbd4a2ca5ef1756258384ae74ab6cc74c238ef9d92aa53539562ce0d226ec2a5a2a5a865c5202486965646c9aa9348edaa4b275359b8db2c67522e55b</t>
+  </si>
+  <si>
+    <t>2019-10-04 00:08:00+07</t>
+  </si>
+  <si>
+    <t>2019-10-04 00:11:30+07</t>
+  </si>
+  <si>
+    <t>2020-10-10 00:00:00+07</t>
+  </si>
+  <si>
+    <t>2019-10-04 00:06:00+07</t>
+  </si>
+  <si>
+    <t>2019-10-04 00:09:00+07</t>
+  </si>
+  <si>
+    <t>2019-10-04 00:07:00+07</t>
+  </si>
+  <si>
+    <t>2019-10-04 00:10:00+07</t>
   </si>
 </sst>
 </file>
@@ -233,7 +245,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -241,7 +253,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -769,14 +781,14 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="28.5546875" customWidth="1"/>
-    <col min="3" max="3" width="110.21875" customWidth="1"/>
+    <col min="2" max="2" width="28.5" customWidth="1"/>
+    <col min="3" max="3" width="110.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -787,7 +799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -798,7 +810,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -809,7 +821,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -820,7 +832,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -831,7 +843,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -842,7 +854,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -853,7 +865,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -864,7 +876,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -875,7 +887,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -900,13 +912,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.375" customWidth="1"/>
+    <col min="5" max="5" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -926,7 +938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -946,7 +958,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -966,7 +978,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -995,18 +1007,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298BA02F-AA7E-434E-AD22-C44EF0C96355}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.21875" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="32.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.25" customWidth="1"/>
+    <col min="3" max="3" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="32.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1035,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -1040,7 +1052,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -1057,7 +1069,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>3</v>
       </c>
@@ -1081,19 +1093,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3FCF28D-9F6E-4A4C-92F3-69FC47D8BA3F}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="13.125" customWidth="1"/>
+    <col min="5" max="5" width="23.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1113,7 +1126,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="21">
         <v>1</v>
       </c>
@@ -1133,7 +1146,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -1153,7 +1166,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25">
         <v>3</v>
       </c>
@@ -1171,6 +1184,75 @@
       </c>
       <c r="F4" s="28">
         <v>70000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10">
+        <v>70000</v>
+      </c>
+      <c r="G10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11">
+        <v>70000</v>
+      </c>
+      <c r="G11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12">
+        <v>70000</v>
+      </c>
+      <c r="G12" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1186,13 +1268,13 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1222,13 +1304,13 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1255,13 +1337,13 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
swq sq swq sw sq :wq
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Exercises\LTWeb2\Đồ Án Cuối Kỳ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3769505-F42C-4619-8B0B-2C45113A73F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65556622-03B1-43A4-8BFD-A0E1D8275561}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" activeTab="3" xr2:uid="{EFC861EB-62D1-4F27-80DA-EEC53D8209EB}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" activeTab="1" xr2:uid="{EFC861EB-62D1-4F27-80DA-EEC53D8209EB}"/>
   </bookViews>
   <sheets>
     <sheet name="TheaterCluster" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="71">
   <si>
     <t>id</t>
   </si>
@@ -111,78 +111,9 @@
     <t>token</t>
   </si>
   <si>
-    <t>CGV Hùng Vương Plaza</t>
-  </si>
-  <si>
-    <t>CGV Pearl Plaza</t>
-  </si>
-  <si>
-    <t>Tầng 5 - Pearl Plaza, 561A Điện Biên Phủ, P.25, Q.Bình Thạnh, TP.HCM</t>
-  </si>
-  <si>
-    <t>CGV Sư Vạn Hạnh</t>
-  </si>
-  <si>
-    <t>Tầng 7 - Hùng Vương Plaza, 126 Hùng Vương, Q.5, TP.HCM</t>
-  </si>
-  <si>
-    <t>Tầng 6 - Vạn Hạnh Mall, 11 Sư Vạn Hạnh, P.12, Q.10, TP.HCM</t>
-  </si>
-  <si>
-    <t>CGV Vincom Center Landmark 81</t>
-  </si>
-  <si>
-    <t>Tầng B1 - TTTM Vincom Center Landmark 81, 772 Điện Biên Phủ, P.22, Q. Bình Thạnh, TP.HCM</t>
-  </si>
-  <si>
-    <t>CGV Aeon Bình Tân</t>
-  </si>
-  <si>
-    <t>Tầng 3 - Trung tâm thương mại Aeon Mall Bình Tân, Số 1 đường số 17A, khu phố 11, phường Bình Trị Đông B, quận Bình Tân, TP.HCM</t>
-  </si>
-  <si>
-    <t>Lotte Nowzone</t>
-  </si>
-  <si>
-    <t>Tầng 5, TTTM Nowzone, 235 Nguyễn Văn Cừ, P. Nguyễn Cư Trinh, Q.1, Tp. Hồ Chí Minh</t>
-  </si>
-  <si>
-    <t>Lotte Gò Vấp</t>
-  </si>
-  <si>
-    <t>Tầng 3, Lotte Mart Gò Vấp, 242 Nguyễn Văn Lượng, Q.Gò Vấp, TP.HCM</t>
-  </si>
-  <si>
-    <t>Lotte Thủ Đức</t>
-  </si>
-  <si>
-    <t>Tầng 2, TTTM Joy Citipoint Thủ Đức, KCX Linh Trung 1, QL 1A, Tp. Hồ Chí Minh</t>
-  </si>
-  <si>
-    <t>Lotte Ung Văn Khiêm</t>
-  </si>
-  <si>
-    <t>Tầng Trệt, TTTM TTC Plaza, Số 26, Đường Ung Văn Khiêm, Phường 25, Quận Bình Thạnh, TP.HCM</t>
-  </si>
-  <si>
-    <t>Cinema 1</t>
-  </si>
-  <si>
     <t>2D</t>
   </si>
   <si>
-    <t>3D</t>
-  </si>
-  <si>
-    <t>4DX</t>
-  </si>
-  <si>
-    <t>Cinema 2</t>
-  </si>
-  <si>
-    <t>Cinema 3</t>
-  </si>
-  <si>
     <t>Bố Già</t>
   </si>
   <si>
@@ -216,25 +147,104 @@
     <t>\xffd8ffe000104a46494600010101004800480000ffdb004300080606070605080707070909080a0c140d0c0b0b0c1912130f141d1a1f1e1d1a1c1c20242e2720222c231c1c2837292c30313434341f27393d38323c2e333432ffdb0043010909090c0b0c180d0d1832211c213232323232323232323232323232323232323232323232323232323232323232323232323232323232323232323232323232ffc20011080546043803012200021101031101ffc4001b00000203010101000000000000000000000001020304050607ffc4001a010101010101010100000000000000000000010203040506ffda000c03010002100310000001f10cb33d54ec8e76511cfae6e21ae600000000000000000000e758740a218eb6c2eae90163403103040d354020000000c4304c00051348301305001269004834c94a125b4ac87118eda6458e12944ea494aa5538c82034820013b18251a11b109c4499092df6d164b6b8035106ac81546c41224488c8aa37408c2c99956e8191688a52a51a94ea94b71584e1208906592ad922210babb674a2b966bcda0d600000000000000000000000000b6ab25d7569cf9ea935ac800000d0000c128020343014000000000018000818a3248804001b88484137072b6d8826571be810c41808922285636856d0324a1292b14930b54a507222843729098cadd77135070850a9454c96a8116d2ea2b708d5b592235df4918a2c9b84a56ac8906c0261657762cf5a60d74f38000000000000000000000000000005dbf9fd3c76c95e8cf6005800000035040008d30005000681a189840000002624ca88d20022681b41294652db1224e7484e0810c473aec57120463257200306b26295c64224e24ca99a259a44dca44a55c967102a958a21150b2708a2dbe899a239e51695aa9d1732a5a2267534531b048c88974e8b552b1111818ba1cf9bac0df10000000000000000000000000000007d3e6f4b1d29ac568058000000d00030001aa1821821800001000a000000c1464ac8a6328006039c1ac884a18304342692b75c86dca2b8d8ea8564100630144349ca762e4348998d7503224e492b4a40c8442ab6ab07198a6d9192092805a4625ee8992aa6152b22545a8ae5280e75a26402cc3ab22a035cc000000000000000000000000000001f479dd2cf4ca49521821820600d5031031300025060860860860860980980860932c88d2201006ad003524b67196691b5994b214a71649a07094022451b489d95cd5ce33272838b22814802b21564071092565a553942712b271452a8ab63199006324cad88b255ca2f5192d2ab7628809ca2222267835ac80000000000000000000000000004a3b65aa17e796be8f3fa4b44671ba8b189808600100313054c0000182182062062000600982681340356449024e28c4d0632521cb6cab20a655d4a75b46a2c684242b24e2d652812db2a59a4a5c4a54cc9918d3890491044e5532c4a068b325e3846222224a5585c216d2a0b6b11271658a100510b1401b824622ca23ab28016000000000000000000000d4c4ad643653663a514cebd627ba8b674ac6ad4d88984a000000310000c04c00501880000000011305434800000934893560d34728ce52510b6a111251404c25107092a40d10dab192a011ca2d4945a322c4ae91955d5a290d451484eb2ae8c489a48915cc938b57192138486c4384c2b538d89348860110dbcce963cf5a40df10000000000036cd6235e4400b19692d328964eeaad96c53b31d79ab4e7df2e8576d59ec21d823ae720eb72800134c01aa0113001f78e034d40144c4134036b1010182000b5cd529ab88a659118898c24a528e404271488a28c4ac90128854301839440001234e69a616dcc0ba5039d446135615d912857333ad02513dd96a09a881af258ec8396714864655251513941ace20409c512946a20269aad9e3d3cc1ae9e5000180305af27573da17dd772f7f22faf56b8d2aed59ebcc5d2ad3159d4a9bc14f439baf3f411bb9fab931d9aecc387a9cfdf9ea6cdf08fbcf2bf4173f2367a5f25664ed70bb92e3cfefb8b67169f43da3c16beff00493e6dd1e77d126bc7edb2e4e251f41f24be4c07402735a5ee8f2fa18e3aa49961a741823b6b4c5a67699d6a73780e953738b26ec7d3c715335c61ebbca7d918f9dd1f41f3f73c3ddd1b0f17bf0fbe3caddd8ce9c3a3e89e2cca7b2e29868f7586cf379fb7df97e514dd4b434e5d11dd9f1ebdbced44e8cdb0c75a2bb2edf9f1cafd19ed8e3aa2bcc211ebf3277d3a2bad777133578bf67e7acecf0fdf720f33d6dbd4b3e69ebfc4fba979997d3e5393cbfa37cb0ae32154903b2b9caebb2b211946e6230d4c31eac94edc9bf3c651b2e01a849aa5d7e469cf6e96cf3bab1eaa7a9c3d5ae1d2b793663d1dacdcd535d8ab992365143d70d9bf8b2cf7dba391337f3b564bcd2ba9df1f4beafe6fbaf3f55c8c1cc3d05dc24bf44c3e46867d9f43c3673de2f1551cbfaa7cafa4d7afd3e26f67dc784ab02c01ce8b467b26fab0c2b9fb7518a579e8d5cc6bd0a28ace84f0d6d756ac75c74d73a6b6e0b63d3c91245e7b3e91f32d3797bba3c3ecb8f611f1171c5fab7c9bb07b1b7c5ccf79f3eaf19f59e1794b0f6dcff236a7b6eb7cc45e44c94dc0b49ae8d753e7edaf6e5baf3d16e431e8af773a5ae3adf3e337b5602e2b563ebe0a66e47d174795cc9a37f183d4757c0d167b7cbe3e061f61e4341f44f37c9c27b1f09bb080354e2131281050812030d6d3c7b164d755e596696bced0a8400201a60d31b8b24d3946996db5db8e9085b0b2ab2171b326fc18f54e23d620495a0021a418289a400440c04c62140626354352800271b81a0900d2608262a601122c09970a719042492173657168445a31351ce6d41db4ca301b88596576a5b14209d6928ce92b8591b2137244e112c5066b5568961192255b75557a126685f4209aa630250638c90020108268430d4c31e959f42631ad8b5cb22d426434c2a82c8d91006d0369927170da92dd3aecc758a064babb66f666d39b3e9aa705be681b681aa18881886900013122d972984d0d0ac4c4c4d0d310c48924c8000c6d03410ae2205e62432c7315a10a0e01193aac922329cd6ab1db354bb09604d24672952275b3170496c2092759146c893828d382492712cbeccf6cd58221a512456596d72894125626818380189495406912112106920675222c69002010589491185a599cd159002c991904e1396d956f3b6e3227755a31db562bb33a41b5aa00a0354c7351188860948443292609b4260a000000c951242182068262a1ab1448ebccd03281a36a6484a129322dd8d54ec6aa49ab1ce581243134849ab191932426267858d295624ae3285017949645211bd99ed94d60c8448add2714961090ac26531ba24538126801a1c24acad4d2449058833a010c4a813463421a189834c54e86652daae5ce0d6c7022d95564ddbab368e7e9cf6d73bda280435600034e569b543162c1129c510d50a48001301a64a9800c10310305215262531b21bf2c648b890ed9aaa7d0cd9e9592aaf09bb26b05385b5a9c1656cebcf56aa2f3b08c12d2a2cb951292c70764c8c48b8045c601172b92ea45728ca41c51645c48c655d84a0aad88e0b2a9963aa4ac5615d76095964044582658464c88c9042562020c47212b00130001803945cb28ca4638f432dcd42352cb6ab73bd524f97bd46c4e90538d836115371024a9a93962c92c06922c6894d1093548611526891254a491a6d62c049b1a1c414d593d0b663d5c58592ebf3f5d1d7e4f3f5db0e9f3e4a2138f6f9baee71e3f4ab94c5c5a6bde665a259f4f1f561ee74f1f2e9bebd79a119c75c5db5cd01a15734224d732b915a90ca251a08a49a112480011293a8b104a20e709c4a70b1453ac6e12231b4285752834231041212486aa4024a48c64a80a0681a70493594e1289ca0d638f7cece75bd1bb3d698dd1e7f4210ba36c15904add91b918e58a9a0131120ae62a699118d9bee79b67b696b8793e77b30f18f77b49af0f1f5bc6b9e13f51d35f087b113c72f75e75ae39eb2b4f3f4fb5b13c2c24a77e8c7462e5eec9a68dfd3cba399d0a79f6d7cae8e4d70a96937e2d78b773797d4dd8ba3cbb9d45f8da95d2a8a3a19ae679f54e9edf29c4b2e5ca301ba9139d325baccd6e75667baa5aa338eb11189052572020608da4b270602101c4251658e364b28a639c6454da2509c082256218670932490a2111b23313080004c0009092c94159639593468ae79d69b30ac6ba54e6d59ef51a72df589828c954531943068006110626d07a3f37e9ef1f49c3a3d0f4f1f1793d7f299efdfe957aef29788f6fe2274f61770355c6fd2726e3bff38f43cbcf5e9f433f7f5cf3f296397ce4969e7f47772ba7c9c7a0e9f2e7bf3758e4f5b97bb2c6a5d3e6dd666d6ddcf39cbe85bcbdd9f7e5e811cb9f4ece774797af36daf572eabac877f90e7585908a0029b8ca6893537646bb11576c0804ee211b92d4ac92544e3621261912a48437190adaec8b5119a9ce8925aa02bae5044e2ac7654cb0ac2b9248109d8d372b02000000001a15462ee5db19352942ccd9ca131c9389eacd767a6ca9eae3ebe43d78ba776985658aa2a691124253811929a454e229262df80b9921cd0e2936641880522cb91089098d29cab664e863d35e0db96e697396bccba796ee7ede6b73df8e3d2cbaf1ecc5ab26e5c5655b18a22af432db1b8d9c2eb7275cd419dbe6a5208c8042072adaca281b8cc9012c6405d5227499072d709477c08ca37001499210c856d762b10a8124e5194aa3622b8ca36218880454d945964d4a183506a0130001a6aab75d92b002719cae49cb394245845c4a706b6dd94cefab2e4ece5e9caf7e1d7a138974c52551b62414866b8d858a516b26a52c54a08464588180c52121126c849083113716d59b703c77dd9ea89769e724e9d18c3468c37dcf475f1acbbb639619d5d7604c4f6f2d31a6fe5bd73d7808ebce096fce365cc54924472a8a9245273962a529426961194449c6c126894e3620482620c4342a6d10dc426292b9d72967149545ab90520013290bae6525294050014c1430002ba8595dd6094a5724e594a2e5938cc938ca1d2b16a5aab96b3395728d7d2e36fe5ea913af3ee934da9baa4d00d22ac454db41a4ae2da42631466950da44121191512410271425144d42b66d8d51bc6d2a6cdb2aad96d9e69cd58eb9ba109d6c2838dc1094ae2b8deee68aa75eb9960ec138834813404d05d9af2e192d621611bd1446c858c704714ec509a4892488158da7280034d4630158b07612d4ac8d89a48084cf6c6772d866a114d828048002cf657a96c872a929034e5728b89ca02cd192c8d6def0308724166bc7767a76a397779fe86337e677a1a346292d83d39e98e325ac21b20d822408912c63276409c510e200d1c1b210b69b8aa2e3bf28946f293834b675b96738b95bae3357570565d582488ab975ca16464a5736465158c9c88bb20111094a6576c59728c46a312d88e5ae3bf1ac045c9171a716d10451c5b48920436a9c99156ce5ab44934576462a528d901a66205909a6845c46c0620627289d7656d59649a72b612834394424e0c59246b234d006034b39d04ba95574dc3a997573f42199f6a9466d4b6629e77041acc84e522c1b4d503223122da04d224e555b622a6ecd715c5adf9209ad70138dccefcd38bd2528e325426138834c210b23645a90c6c938465941c6c26ad23152224ea2d4406a289c881a73b8cd4532e529c2c6e32224e456ec52d448b2249c3b616ab94486958acb1ae4af5d0944265cd632c438c892958c00060042a6caf5264a3126a4ac4e502049c643a2745cb69ea0d289252a4c21b4c9dd4dd9deaec717a5c3dd9a328df529c6458d99e95494ac8b62a6000034c4315290442490692226acaa9bcbcf247453ae35c670d795c5ab857577b3285b196a4e152956c915b59a40e5143945ca22364d4895271ab128929a9224e24eb1114c2508b24a258da2563989889a44a59531265919bb1116425055d4eca2e95d9115d36e74493b2044654250b972004d0c1c09c6ab6a7602712639a00156dd9352a0809dc8050c20180d3094644ec85b9ddfd3e575f8faf1ad5967b494276cf464bf3aaa36c2c18d536e589242262c1828a4106d228c958d38a414ddcd7468cd79d519adf8a0386b94b465b934d53cf041949388324ad4d4d464035625aa332c725396b56d682256323525d2cc8b942c948d950a23d65324b125642b01623222a4ac14a52d737248da31d6584cd42c6035aa3352c71ebcb6569c6e10caa85273602a006d395c250b14924535256d39404537533b95538d92028610000c01a06c64ecaecceeeebf1fb3c7d52cb618f7d2e74ea493ad89cebb61dfcd2f1d73a6c84efcd3d76badb409dd260b11e1bc9e5cf2edf2afbb009da8f33a3cfdd1a7456d50a70d79926b5c609c6e24c051d329734b4456b726dd6492ca5394b4ad374bce76c6c5344a4546e5c2b5ae555761ae494a203817e9e7d937717d336d8a57642c149031a2b52115d5dc36982b5a669d93256c653508c86a9aeea5566baab8ae43b2d223586717780d00d31b4e58c5ab1d73aecb24a52b07295594d845ab121d803002060000301ca3259db0bb3bb7abcbeb70f5572bb3f3f6519afa3a71b0aadbcedafa99a57eef9bd6cf09f1fb31e53c05127d3db5291aeb16c56ea6d4f9dbfbf7c992d5e89e6f0dc5fad72b58f9bebb70749d6aadaf97d1ae16c75c2885d4efcf192b199c5fb5cebcfe9f6b2e7af9e62fa5f9cd4f38abbeef29a2c7583b2b95684e5c099bcca2492ba3560d70947a7dd98f250eff0026b355b6cb9e71a336a3134b3663d59e9597d5353b6b915b0244995ce700424b2dcb7a6a50acba144d7518e535a6141372adc48d5386b11527648913ae212d7924206c60c52c5356244ac9493ce9802cf7d172e2d58a43a01c218260002834926a4b29c6eced77397d2e3eabb3ea38fa70e7beaebc2a64ef2ec76397eab8f5e4f6a79b5c79cfa94675e532f6f8f7d749335d6b141ce5643b4698757a33c7e4bd239eb31e11ba3ce794f71e4facd955b567db184abd79e099be2465df936eeea2e3d2ae967d7995e2a1dbe4b91e8bc7f6c757b5e6fd3f1f6ebe6ebaf8f5a6373de38f61676e5773fb34637cecdd1bfa79bd349cb8eeda345ccf073f6f9bb7988fa19ea78fc9ecbcbf4e35d13af78e9462f3d65384c52884dc02d8112294596959516925d6536cd8d134d35371056421385ccafaac9d511275e788ebf324d395b52948b44471b95642c56d4a54a5115175172d4a36363006a26c8b0000018a4a44efa2ec6f7eaa3a7e7f752b6cb8fa38f0e9e6e9c30eee6eadf28fb6f11eab2ea64ab9a9e832c71e37572abbb5e98494dd638b7e2bc6cea71fad73ddd38704f374b7f276eb36d3d4a263c9f23d070afb68aedaf56baadab5e65125ae4fe93c2f5fcaf86abd9e39adb54b818bbf9d0ec6dc4f0df43f9ef6e3a3d3795f51cfd1a7453abc7ed9d3dda79f3c4f7c98e553d32efc57731f7bdbe6c70cf2b8f4f7e48f3d59cde455b9da5e7f72eaf27dcf3bd39e68b3b79f72b23cfd088d765ca977372832c2b6ad26ca95a1091296bbaab1a22935370734e0e36029aa6467699233d39728cbb7ca6d4a56d39520455d95ea592529a6d3c9265473df4eb2262390d5360860860868001b4c9dd55d8debf43e73bbe6f7e85ceddc3d3a70743b13cdf3f9fa697a7cfcfdf5eb59c29e6e35d0c5e832ef3c85ededaf234faeab53c8737dcf1a6fc8f6d64b8f49c4ed5bcf7e5fdce5db79acb6797cef6702daf5eca216d5ae7553a2ae9e6539b63e85d3cafcfabd73a8a859cdf519d78fa7dbf3f7383e0fd878eefca7ec7c77d239eeadecf9feabad84dc7373bb15eb59f4695ac72aeb6ced78b575ecde5f97eff366b9f57a2f3dd79c3240b67cfbb2ef946d776b3329963a592d15c519ba2ab04e65b09032e718d96a8a4b20d2b20964eb26a4e2d5c5ab5d8a78ed539274908979cd4bb7ca249cb2025516ac494d2524e69b14a80b2bae71d662c904872a1803403421821889813b69b26f47638de93cfecb7ad45be0ef6d909f7f365ade8f473ebe7d593af18d95cf3bdb379fa72b31dbccd5d2b3bb6ca72425e15bdcc5c7a723d1735f3dfa4862973df2f933874f528590b6961785709437c6e9d5a98fa0d73f2fc35e96af3fa36cdebfcbf6f969f1a9c96f2fcef4307b3c967d13e7ff0050f377cd7d7778fbc3564dfac5b4cb3eb9eccd42d1e8c36f4e9b32f1f759c7751a77393e93972f173558fae21547d6eb971e5ebe5cfa78bea4b9baccebceb53557970d975555bac7462aee7df33ba1ae5069128baa926c131a1a72c9b9ceae4cc7a60e42c098729a7dbe449a9289c6522d591babb06d4a57194655116a406ae54938602b63953010c10310149823ba9ba6aff45e7fbfe6f5f72ad6797a470677e9e1bfb51977f3e6be658efe56c2daa51da8e3eff2f6f763cfec13b2c671adead39b81d7b38755cce9e5cef265eaa5f395fa3e2cf4d145f1d73cd5dd56f8ae97376b3efe986ee3795e7fd061dd2abb9b2987579ddc86425e8f2743e99e03e8be3ed0b9ae08a9d52bc3bb35e99217e5dee7af2c779bf91b4d3ce4ba98b73d2f9cd9e7f37353647bf0eefb3e7f5fcdd4c7bb066e3e5f7f85d1c2cbdcc1d33c7cbd2e7f5f3ae8e4e94de6d3cfdd35667be0cd4adac88a54a4e53517626a963594a067d17919e7ab639b430e331f7f8d269ca90ac149126395c93948ca254d1ac8982630025934d4190861119609a04c1d95d92dfdee177387abbf9658786f4e5bb93df8fbc9552ede79c285cf7b6b35cc510793b5e379d25a7a3ea65e9538df513a4ae590945b410cdb34dc988a94a2aa753ae6f88fa6792cf4f35d55d1e7db6def97974393cba7a6764b046b2722c3b79a3ddbe78deaf57e77b7e4ebba595f39b29a2bbaea510d5d58795e93936d38368d79be77a5c3d671a5aa3659cfbf3a55e8389ecd9eacfcdfaae3a9f3f5f0a5e872dd9bb878fe8bcfea62c3d1c5d79e9a166b2beaf2faec46b509ab6b57545ce32c5a6b2073a44baa9da2d13564eab6749c939d018715a977f8b2052a4cb236c272837000a45c6a00ee44c131ca98c724e5060936446111951608ac84e5d1d4e4efe5e8f519fa1c5e1bcd0cdd6efcbd195e5667170e1e8eb5fcf7be17f36fc5d2717663f41d33b2eaa5d33a6b2896ecd5b48b9c086dcbd0ca688cccd3060c5cee9135e47a564787a2fe1f6f9935c1c1d4cbdb9e7b1e1d63bd6d71e76ee4efa5aeb4f9f673edd8db96dc73a77f3e9e92cf55e5fd575e4537ad67c6eabbcd73f476f2732a9abb0d39ba66cae32d63d17accbd6f3eb16b71cde6e5e8d5ab2e357ab7179bf45c2b39f8f467e98a2ab2be9c2ee9e1bb3d088d2332b5b541cb39536b765b9a79efaabb258f5e695d14aec936a0e511910e4493eff15c5a944dd9269e68d49442126aa0d3b960e54c62639642164294252421ab129045328945c5da72eee7dbd479fe9f2b975a3d6799f5bd7898ece773e9b7662e8e3787a14bedc27cee879fb33fa1e374ba62fb72434eac7048d51a11a239f661aef85932557245646542712c104b9dd1e34d61bbb59b9f5f3fcdf530d3c4f6fd2d9d3979c7e8b3472b455d5e1d30abf2f495cf35ba8a0911f69e43db24c74dc51e1fded58e9f248aaba5b54452fcfd14fa5d544fcbd6caf9897b91ba2ce2cd673aeb165dfc7e939f47a6c7a9cde5fb8f3172ab8c37ce5115ccc4d66326872b33da068967d259179f45846ccf4aa528d894d9593138724fbfc3516584d3946886d35516584440d30639418036263964372c49222a6ac8a9222a4ac4d48bb5e2bf1d3d073acab97a3a5dcc9a7af9a3c1eff2b3ad1d2e2f6b8f7ae1653d784b85d4e26f3bb572ba9d3103742b03b73c2b2a866ecf43877c929433b3ae755c10b68273ae4b38c9592e2f585ae560889531351919e8df35e7c2ccd9dc33db5564a6dc1a6a9d16c4fd878eeea7a15195c9c8eb878af29f5be6ce9f2c5ebd5792d1dccabecb1f469f3f5e3752aaadec554e5ca79e31d28aedbb79f3957ade5358b9f9f45ce12dafaf994cb4adca53516ac9d2cbcbf9fd0ad5919d864e6a0d8a0912122402f0d38fa3f3e992b1a0946a4080232889a29b4e18dca49592d526c4294b36dcb056448128d91538d894a362044edcf6cd7522b673ebe81c0d72941a9793dfe46fe3e8d5ceeb7175cebe1f5f276e5b274ece99a9eb89861a73e2d5d3abd3e646aa6eb324b0d1a7a7b134745f08aad8b96710b2a9ca4a488254a245aeb996d70ccb5e69519dc73c69d218a6e96be7ec2dddc347d26daa59ccc8bb2324cc56c2e9513761293d66b7549542fcf9b933f52f5f21a7d33ae073bd873b37e537f7b978f564a77f377e78dea7bcd603529475e3d16c93e7f462d16d88268004a6922d163025e220f47c0249898400e84208b5434e1b5251844adaf467453a2acdaa4edb19296755c6655519ab2319c6c8a6ac8a92b14e161afd179aebf2f476e246f19109b5666bb3e3a7673592c3c9476d5eae36e8af5eb39d6c866e7ba5dcc2737cfd6299e7ccb2ea733a275a509580d4563af36c9c5595474d4590ae6b593919ddc4ab9bd4e32cb25f8d72d70a348d13aeacd98349679ced73ae7e932f9c7d0b96fb8737633a082d66a7c3d59deeba8e159eaa3c2e8eb33ab4e5ceaed1cd82ecd386c6763cd66f36e37c4e5be4e2e374f97b2bc97d3d7cf191eef59f3dd5ed1cee43a16cbe3f8bf4ee06bd5e44b14fa3162134329b6a86d6201c207e8fce8d35001a412838809d0c21c94a56352cf45376752719e6c89525869a4aa365642335508ca1acc54a3628ce3646702b575b87d1e7d7d2d5cddd95b6551974e15c3d3d5f4bcef6b16ae17a0e7695dd9ba3db853afa57e6536a824bcff5b856eccb3cf2d7e9bc57d0316d717bc4e2a32baecaa3456edd4cd1d19a55a2bba146512b9c2c31e0d7926f315d5a578364ab893d18ac8ede64aacbe98a55d6e7f2cfae4fcafa8e1d25571a0bdac5855bafd178e8dcfa0cfd5ae5e1dbd2cf34b561d69d5a33ecd72ad63eb1c7f99fb9f1177a3aab679fd98ada35eb8f6fabe7ba1796bb73686ac71b10d34bb8f23c9f63e367d7403d11522e41a518e5430f3ec7e9fce2001348c22ae2d5834c6d3964e3295b096db2bb31a9dd5396bd78fac6dc3d0e773ed96ababe9c2b8cebb6109c6e62a51d48a946c8a71b1e8cd397b367336f3f439f2a3ae7d4e5ca1acf5fd1f93f43cfaeb8c3a58b5f4ea9f6f34a31823a1e7968e66aa2a5c4b28e5d3bde9f2ebe9ced4a94b20a997614d8591a0abe1302c4040a624e8ccb760d754d4795d2c954f37ad1d39f5dd9ab9f2c56eb3054dac965dd69ae17433e33dcf63e7bf42e7b9472f0f3ae9f9aef67b6bf49e1fd7c68adc63174b8fc0d4fa3537d9337c633b8e67cbbd67067a3bfa73eaf1faf93dae2fa2edcbca74fab9b7cf9cb87b7af1f41dbf9dd527d4a7e77d166e7f07eefc1e7dc26afb49215b09a4c1418bc04d7a7f3402188101611686e321b5295ca3295b8ce59d909e7575328c5ddfe4fa5c6aff37ef3c4f3bcfaaea7be2aae7014651a51942c51947598a71b09d723574b95bb9f7c2ba79359a699c37cf577bcdfa4e3e8f43a6da75e673ae564692894caf28b9857cfa537e5e969ec6caa7be450ea974517572dd5e0af97a39f6d4b4f47bfcafa5d71b2253ac3c75f32dbf479ff004ca533c79b6c32eaa51aea21976f1ab911a9f4e73d557a29ad3a679b9eb859b75da9edfaf567c32f92e45b75d7d35dfc3d1ce8746166594f06a6fb7360b3d5f5b2d8e5d3cabca2794ebf27d04f64fa1d2bbcd9e3f574516434648eb7cce47ab7bc7038fb79dd78e9f79e43d74ce2f25af993d5a1ab73f460e49d0001a164225f3e07abf3421008b012418a9b5295ca3295b5294b2b9e6cedaa534e75694e87a2e2fa2e5d2ff2bedfcae71c2a6fcfde549c6551946944561094359516ac4d1659af15d9df7799a6be7e8e5a677f23fa2f8cfa1634e98d5336caa999b1dbca5b38d5579d68aaab96cf4fb74eb329c64ce48d739abea98479ddac3cbbf0e8d19ed7d4e361de3e8bcae9bbcbcce4f434f494f574e2e778f93b326b9193bf86b06db78e9d1e22c1a94caaddacf4ba3cde8e37b39dd8866e4cb74ebab5f336c78ef47c6e9cdf62ccd5f9fd1a634c2ce8e6c17d9d2c496b3dbe971bb77951f2bf47e57ae75f53157cfb6bd1c7bf7c3d574fce767cdebcd406e6ae9f3ab8df9b56dcbcdf0abc5e8e1674724f3eddaa1673fa314caa8955785b2cd616158d71817a3e089aa4090116026394652b9272b612bb2bb33a6d359eccdbb1aed75f85d7e7adb9eedce3f36aba7c9eb611956ae2d58a2d5461386b2a328d8815929d5336ece774397a390fabec7a70e7f6adc7267b6a966ce55706a3c3a65a97d51d7351d3675b3d3bd65365e3638c0e75d8f5b5a6338c6fe4f5334bc1a3a38a74c1cad79b53dbf4b87d473e953804e8e0b7919d1c1daf5735529ea435ec9cbcac1dbb93cdececa326f9d52bb6ab8cab4652d555e72b91ea7c569ec67874f9bd366ec5cf3afc5874359a2e9f7f59865e3795df2ab663d5b9d7e5f472f3b08d7dbdcebb8e0f37abbd96ee84bc2bbb5cfb25e472e7ede78e8aa7b96aaccf4e94f269e5f413cf26af75a7459af95e35998d70c69c7afcf111b1c48d925168da6b29272b6a52b689656573cd73aed9abb763e8f2efade7af1bebd7cb3a73e879beb7335ce84e3acc095763446c4a4ac8a946c5171d65ca122fdf87772edecb779af4525b9eac5ae738f1f836f5b8d0e86a73e4992e8f3fd2e3acfb9645876576b33cbaf9466d7975dd6dae71cb42af41c4ae5b34f03dcdd9eb3e6edf1e5ec753cfda9dec9569c6abf3f0dba73bab93a2938bae59dd5c09acf03a1462d85b6c025cbdd517513c43e3f528d4e577fcd77f1d37d992ac6f5613a35d2e9ac939fcfb1d72f472eb570b79f6d38eea2e29f57c7e9f3e9aeae3f6b1d29df54a5d5e6a9d3d78ae57aaf2bbca85da1613aac9a4a102ca6abae6cbb1cb3df6b59b1ea999cdf931a71ebe349c6c438d0269269c4a5194d36a52b02594e139a76d5a33ad3d2c5afcfe9d55516e379abd54ef34d17c378c50b6ae9c229ad66235628b8d89356462d6b28689e8cb397afddf25ab977d1c84baf9c029b884e74d99d6cf71caebcb6109b3375d859c3ebf9e5d5bb0ea5d909aca3bf06c383a69af4ab97d0e6d6be973366751e4753b49cbc1ebbc6174b6625d12ad8e55462c2ac15a19cd3a3bb3e73a7572c3a11c882a8ec2859bb6b6fb5a36e730a1e7cea9d17c25a2ad39cf92edc9d6ed9753c79d3d7cddbd38f73b5caf41e5f6e3cdd8cd9b87cde9cbdfceb6658f5e3d1bb97ddc74f3d65986749199eb9cedaee96545b62d17c252d79e75dcc898d628ca1bf3882945ab0698e51944a5194d37172c80965657396cd346ce7db5c9d3c7b572adeb33bb2b96f8422d5793563ebc14650df2110b9135628b5a9113b04c094665b767d1cfb2c9d2c1ac400d6251406dc5dd97d75373ca8d39606db68228e6e9c9abaf451aa1d99652e9b79b612c1d1e2d5bcddf9ab677795ecb28db9ae4e1f27a5c39baecc51add0c732746c665967cb51df884dcb9d59d2af7fb1cebc7eaf576e2f9acfea4af3de92db999d7357256b36752b2879d154f3b5f39afafc8edc8a6cab788df4db46acd1976cf97a134928d3a1ccbbadc7df9d6cf3becfcbf3ebceaf7e6de079a766d52cd9ddd4d95591b62d2824599e328eb99194488cb134c6d3894a3256e329a6e329653aeccdd3bb26ee1e9d3cbddcb8b945ea3625941569666be8d62316b7ce29c75922e361171b2235632224e754d6fb69dbcfb6acda78cb06974e1269cd3ee713b59d75bafe1bd75cdbcbeb55242ee3d8bbe8bf29768e7681ca9856a8460bd1f37e9fcb9af45deaa2c8929199f9b9b671fd4701bf2b0bacdc8d1d8c92f3b1752367329eb5166096e8141d3eb4bdbf4709cc2a2e52d0ed8e6dd0aecb1c63cd974ac5ab1b33a16ce06cf276f4381def39d79b98f7ceda932d83910aee6553b6548530d7974cbd9c72d7cba79379baba6135e72bb4aecb68b194d76d57322c0c89bb98c651b220ac0024e328938b5938b964d39656576e77bb7e2e8f9fd58f0ce1be522122c558ac575579efcf70a2e3be6448d89376415caa88e88dcd04e08dc555da30cf3aede1a3a38efcd90f7c13b89ad3d1c174d54155cfa8d9e13b5277b3ca650f54ce3d98acad6b34d6fbf9ddf89707b9d04d5a2354595ca30b93d2f3b9e9d0f2d2bb4c9d3e57597439db1cb9f5207117a089c93bc263f4fe6b875f458fccbd25cfa98c6524064d428d1933a960b754b80d95cb1aaff0022b8aeab4ef2b85e9bcd6b2272e9ce229129464926a630628b4597e3d0bd1ef79debf3df9633e7b75e594ae69d799d96974a6f358b3336959735cebb6aa84ebb95169189d3719127172c9c5c49a7353baabf1d3a364f91cbb094ba728c92272adcaeca52df93466b08b8ef928858e716ae2d08158a32572a3644a0659674b2ebe7db2daeb45ab2c8e9c74e45aaab29b95591b37767cdd47a433425d9bf34d14b48af765cb97a5dbc9eb228e5b73a9591a8a7174f82be735fa7f1da6ecd8ba8bd2dfe77a19bd59d2f2bede76cb2dcb8ba55cbe3b9b5c83afc3dceff005fcedd97bdbbc0f5a4f498b8d0ceba50ae39d697cfe20b242fde65b2ad7cf79381d1e776e2990e987642449c2c494e122522b5288c12edf8b62dbd6e36cc6bcfcac5509530b35599e135a2ca5ad688dc585a4d609465ae70ae70b22058c2e8a89c09022528c95ca2e5b3663dfcbbece3eec11669c4f59d34915938c524a2ac93858550943591c656341280ac693449ab2437359cbb4128d56e776d56d79d42ca77eb9ebcb7672354a3691e9f3a74edf6343c6781e6fe8f86cf015face46f3caecf37659e8b9f5558df73d0e6cdcf5d679735ccf3d75db6579fcf591e6cb674c5af9fbe5d7b31d79d7737799d52f7f996e294edf1fab356f37bfc04ee64bba373e66ea7367aebeef97e9276ebcaa4d151c2c6b0e495dd11d06ae5a942df33ac56d1e9e118825aa51a77576156de7ec2345d8914a16a6d77c26aeb96fc6fcc4435612065d56140a08edab52d24831345e718ca3493564f466b25820b18a50dc5ac9a72ddd0c1d1e5e9c158b7c66904844b28c4b1ca0d1348b29baa20e26b3301534ac6211a1939ab31d3773ba7825a2507ac6850967a1bb0f412354abd660935eb712dab3bf75a381decc9e6d35e6b35d72f0f97ebe9d381dbbebcd9f3de595d9839fbcf772f9ba3a73e9d57f56bccebdd9936c2eeb65cce8caa97166ec25e15bab936757b9e17b59e9d2df973677af571fa92be274769c9cfad637575b95cfd67b7c8b2dcdcfa2f9e2c26bcf5cd796e8fafcb07135137134c24c84e200e4979777b974f370ed72e8aa376f12e83c58e9cfaadaf5111763698eb9c435d308081739986b3142b00000006124e06259ca1396fd99d73f4e59d6fa79e4c52ce2880458c1ac46872ae4421696446090ac6444728b2eb6a9e3af473c9e35cd61d793957396cea73f5cb5533aac838d8a39d3372f59e3af67dd4f95dbc5d544f04bb72db965b31ae64d67860b77978b5f3b79a6537be54f7f8703dff003f17a1e7ae55d4ccbf4e552eacd6dcbcfe677ef3cf63ee726acebf99e963af41e3c3cfa76de3d39d315d8d59c8e8f137cfbd4d91e7a22713595cdb21ebf2c6f855a8d5a228a2af8d617406929d7d9c6b742dc7e5fa072fa674e3cee9766abcfcce7847b739a5a25aeadd9160e32d60aa71b96d48808295285ca5211292a4c0018038600edaeecef5e1e87333d589ef8b526a2e8f3256023710945a0685716aa446c2119c11215cb9d732dba8bf1d67d3e5f6b9f4f3d7d76f4e58e70773aef8a5aebb29b174f95a26e31ae6904dd3edf1a897e88789f439e9d1c57d3961e377301cddd557667aa51ebc549028c9595fa0e1d527d0797cff0043cf7875e5cd5b5d99b2be74cd5e1d6a5e3c35666f54b35fcfb68b724f1bdcb2bc5cb3e47a4edc6657c5e7aea79f9bf479f3b9c3a604a48ad502eaaf815bb0486ccde939f5a3af9aaf27a68cf52ebd77df9f6ce57f9fd7e6fa72b2b81e8f3d9a71e9ceafcc5134cacdf293895375c86216a8b6c83424c488ca27022400a51912d346dc77973f56512b0d7352096b62b196d24a23126914a3259212965560576d6406ae094664acae79e967678bd4e7db994dd4ef834acb3a19a55528b8114d592d19efc75cfbe8a9ba2ecf6eb91af1b5f453e2ede7dea85f999bb0dd8f5cc4d6f92716205609855d5e7551ee5791f478d4b7146770afa1491ae376758a3b0cef34b4d99d64e85d388703a5856155f876c45d9fb79ed2b9b22688a93b2ecf6d45d1956595c674fb1cd972e9d4cd8e8c77d9ab9bd6b76db6f98c31c147d3e4694ec9cea73444694b1eb0db26902264c9ac76512d73b13628c909a68818371524a64fa38ba1c7d5caa83af9cb2b984a24b22025954a548714837124e22ce321aaeeaec65d738cd56a4b5cd4e2cb251967a4f7e1d9cfb47075399ae31d55ad66ca914e033a1cce8f3a6ae2129d35513d18f47256acdd7c8ee8df12d59972edb735659453a7375e0991b89496d9d702b2579e672764512299b82763abe46dcebd6d5cc963a7a3b3ccedc5e85367433be7dfaa98aeccf88ecf0f5e2cf5cda6fe9b5e36b9af4f922493298964c824a28b24a72236a92d118c472806ef4397adc3d1cbf3b666ebc6c837acd7642764650076ad99df3ade8519d4b1f4f346459afebcae224d67aeeaf788595366f55590302328cc719257385b3576aace5e9e701d7cc37296a94e3511c124810691351090a4a31b5558866642c9aae338dca6165813ced6dc7a71d76f27a7cf7343a7a60718d8c883b216e7751b7017df91e7ae8ae333a1cbb629a689296355db2b26591be566ce74648ebc76d599dd82a88dcc6dacb2c8c82b564504e328988a71bd60eea26a91bb8e87a5e6fa2f37b3a1ccea79fe4f3ef54fbe3937745d99b5c6ec6ab8e8b65e7f3fbaf59f3d66ba7af3586ea6c49ab1f431fa8e7d6dc3ab072ebc08cf7f7f37397aae9f2df87d9eb30e7bf98e8abf5633973b2bb167b7af0ab2f6399be57d9d4e7e7759334c7070d7288d584a217945b05b0b160c617d5a31d3562e871b3d403a79cb2519b6d39650b2b210b1dc56e4aaca3766ceaabeb7acc3adcffb259e057d044f032f6f69e078ff005af989e78416d955d8e8afc9a33d3a3ceebf159840875e328a4128db352b2a26accd64514b6e2b55c2cd94ec9e3b5745d8f7cb67538faf3d7aefddd1d3cbf26a7ea7559e3f67b9d27c9791e87ced26451b051c42600a51b22294413549492138eecefb9d4c3bbc5edd3e5fa7cadf2addc6f2aea6f216252dee8b62e9d3696717a7c2d4ae1757d715962b9e9687472edb6ea6ce7be9ba23c3d7a72e08eb473afc1dfcf3f4993b39caf3bea38f9d7977d7c1dfcf1a5e3df2ede5c9b5a89317951947a79c18252421a2db72ca2f719acf453a79f7b795d1e788db8758d71aaf9acd7d7b66965f49e91af99f7fd2cb7e7f9c29d63408590dc69f79c9d965be07ddd478af770acdbf33fa1527cf51f405f077fd02c97e6f77d0279d78ce37d36aaf9a1f4be0ef979023295dabe9135f343ea2acf984bbfe765b2032738fbccdf218be9f06be5d0f49e6f7caceb73bdacd748ad5ce98d10b3660ba47cc23f49f9ccb03e81b2cf9cdbf4533d3e6757d3ebb8f99bfa72b3e64fddf84146701b9f7b1e8f3ebd0bcf6f3fd2c9d170eb68c0bcfefa896dd672d1a29be750b26de6d40ee0c8be10aeccf9afa3a792b8f4ac9df9075b35983a1cfbb5e6bb54df2f76ce4eee3468557a472e27ab171efa28cb4e3a6cab369b8c75db474e3c2afd264efe6c0f24f78d6564d73e13875e081a21a01824e23ba823a3bb91d9e5e9c35d51e9cba35e7bf1d31b8adf1b36f36737eebd470fb5ac68c5a7cd9e1e1bb073ee9c63be32fab7cfbea372ae8cec8d3756516cec23e7bd278397c9fd9be65f50088ac719c4ae530afc07d0fe3e60b23d1c6edfaefce3e87638c56b3e4fc07d3fe693555bd6c79bdafa3e4d5ac0d42be59c7974a5f7fd955d96c08938a8174f06a38bf35f59cc97e953ab459085a14db39151391e23c0fa1f3c45346fed61d9e7fb4e0f14df3bb7c3eeefe5d82397d97d2e7f4e639f93453af9f73167eb8008622646a9c57d3d3e4f4243e7f52187a1cbdf928db8ba9bf2e90387d8a78dd1e7f6f9167b2f25ea794d1c7d9cbe5ed8f63b77ebcde5ae9d19dc73e8a3584e9ab588f27bf97af2e481db8d29abcc14a10d534024d0c6e1f5399ab3d73592cfac5e4d63a513adef9464baa7d3e5666b1790f6bf31c75dfc7ee61e1ebe4573abd1e3f65edfcff00775ceecda7c896dff3af419d7d1d8b59b3e53f4bf904bddf47f3d4bf5ddfcceadcae6757e7d9d7721e2e9c75f5fe01be9c6eb953cf7eff00d5f37a5d39d52842b27cd3e9df289757b3f37f48ceaf8b5bc3e07a0f0b2f8ff53e57e8535e96b25ac64f3cbc0cbf43effcefea566296981f32d3c6973ededfaff2ff00a65c74884b78cbc8e4f99e7dfdc2f9d477c6ca5c6c0574bdcb11e6fbc72fb3c1df9abeff0007d05e0d4a3c7ebcb6e257c392caefd72b00c7d38d2477f3acba8bf3ea0233b609e7dbd7e5e86ce5f5abe3f4b9bd7e547b7caeab64a2f9fbf975c2eedf156dcfeb78f5a232b78fafb690e1e3eee7d9d73b68166d05f1d6299146b3619cd679083d1e4728cd44d4241624c24c9416434cde48ce761bb9f3ceeabe0ec7eb7ca7d0cede5dd1d73e7fce7d878dc77e8cb9da38f7e5296fefe4fa76872d623f37fa5fc64abdc786fa7cbd5159670fe6decbc54d4b464f4a9f4b68b0f947d2be61cfb38b9f3f4722faf475f248afbe7d14556f1752ee33fcdbe9dc895f629b51ca4547e61f4df8d6774fd77e6bf53b98c6659f3af37d2c19e9ed7dcf9fec6b9ddc3ec78e97c8b52e7db4fd57e7ff0047df2ae36e0b9f03c6e8f378fb3226bb791271b0df83b38f46d4d79fed4b9b6f3ba7cfb7b9cce8e7b0c59f6d34c16fe3cb6e2dd9f5c494f3eb7dcb6af378b9597467f47b0a2fc1bc51d2e6f535e66e32c7bf9f8ec876f89b3766d3cbea14dd88e7db4beff1aef5be47d679bd75f7736fe7d659b470d8f37cfe9717d5e6f52727b1c7d094a119f3e8a77ce9266b3c503d1e494a32945244071b09466126a596dc53ceeea6d53a515d95ef884525bf5bf997d589a92b3c3796ebf2f9fa6b90ae2bf5de43e93ae5dfb2acf655f29f71e26587d9be5df4fb2c9903e5fc4b212afa0780faf274470af37e37b7c5e1e98495b9efcb751dbc51fa07cfbeb9acee8a76325023654cb2aaab355f4cce17cd3d9f8ecefd5fbdf3de8358399d2f3135e1a6bbfcbd7f4194a3dbc51f99fd2fe439dd6c58d7b9f59ceea74e6bccfa7f0d35e633ebcbcbd18548ede580161e8b89dfe3f458a5cbe9f1f2dd0f47c3dfd0cba387d6216e69acf14ba7c8d7aa9bb9fd735e4d38ebd48e0d5c38f2587a3d0592f61cfc3f39ddd3e675e8854eb7820b476f91d19870fb672babc7df8a92ea3afccd5ebbc3fa7e1dfbe55b38f6b3cef7fcbdbcce3f439bebf1dfeb3cc7a9e3e9ab26bcfcfa67aeea77cab206f1c869fa3c9294652b40b18ce29169d9738599d434e7e967a18efcb9eaab9ae9e7e872f4dc76fd9f03d36b19ee382781bb2eac7618b1d2bfac792f5dbe29eb5be7cd8f5a662d1a2b2ae375fc71e2dc49757d97e6bf4db1c5f30f9c983a3c3d51b49f3f470e21e8f05ff62f9c7d1759aefcdce4d7a3cdfa21c27948747c6fb65a2f04f96f1a5d39afa55f28dcd98b4a335f749675cd59c8f9b7b1f1dcfb46e877a3e8ac7d789f29fa57cb39f5c10ba8a4a659429c6e3a7d3c7b3cff006e2ac8e7d000c886aa4a4b57375e2e9f2fa96e1ddcfe80353bb0200d926be8e47e5f371f387afba09688180d4dd7c9e860ebf29d162e9e2afdaf8cd5cf5ef2ff00196f9fd7975d98f79e660d19fd5e2d3ec3cdfa3f37ba9ad68e7d7166df937c7281d38f1c47a3cb269ac809484e245b2c7384a25ab2dd8e90a255eb2e75eab2fc77d935f5192af5ceef0decbe6661bb3d99dedd5cfe872f57a5f47cceaf5f2ecaa8e66b1ddbbc2f48f44a5029f9b7d47e2c5604bef3d5f3f7d97799f47e2a6bcbefc9a38fa34db5ddc7d5e69db47abc1eefd461e8eb9d5e57d4f842bf7df2cfaa4b678eecfced7d8fade3762e5f1fa7e48f1beb7c9fd126bd2c651b851e5f3e6bd3d7c6efd955a493e71c5b6ae3eb5edfc37d4f7cbaad1d38f9af09e87cc72f43c7a29b019652ac2e3b96718e3f53b271a4df5973ba19eb21bcf74f262df96667ea6fc5a44f8fd80cd8f5e6ea98374eaeea279d6a7bf97c78661aefe91596ce79dd955d0d0bcbcee5dfe1593b89be7d7655bf38d3b1b80ba2354a2dd3814df63779a31d7d4e1e67479ef2961ac70c0f4f8dca3256d39406a9b9456c2c77556e7755775b663642e27e97ce7bf3d2d36d7660f96fd0be7ab292db9e95df2d18e9f48b216f4f343e79f42f900bd7f90fa2cdf6dd86b1c8f96fb6f132ad147a23e928761f2efa27cc31d6bdb8b572edaefcb3e5e9c79f6eeefe6fa0ab21dbc8fe53f49f96e3ac3e8ff3ab65950bb0bf470ab7c67f34fa2fc9a6e3f5ef9a7d4d2139d773e0381d0c9c7dbea7db707b7d7cb3e5f47cba78caeea387b2efaf7ce7e8ddbcac5975cfe6f92ea3cff43a3daec777bf87c570bea5f334f3804d8cb26a32999e875b07439fbc033ece664b6beff0977795d6c7b8039fd0e7639d7dfe1f436d5672faae50b337a3ce8473c640b5eab5bea73f0f193874f54aea6535d3d3c5d5c7e7cb89d1c7d671a128fb3c12538227174dc58c8c9470637124d46533bccd1d393945927172da04d16424d4051b9b34e3d39d5128963af4d22fa8fcdbeb9719ad8e7b3caf94e8e1ceddaeacf4afd4797fa0eb9f71599ae33fcbfda78b53eb7f35fa616599ae4f9e702eaa6a3ef3c37d4cea5328eb3e7bc576fcee3b5b6e7b31d2fdb8f771f566f51e77db75e1d3a94bb78fcef88f43cae5e9c668a26a3eafcb7d175cf65c43a70e4fcf3d6f93c77f49ee783dfd72963dbe6cf20a7a78fbfe8b633bfce3c1fbbf99e3be7a7555cbd7ebbd672fa5dfe74bce7a1f0ad799b0ddc7d9f4db3ce2ebe3f47f1cf65e1d60494b1d355d9e93a6509be86aa2fe5f508595b7cd35cb7f2abd95d98fa6e9b72af3d4b476f91d04d72faeea7c9be4ead94db3ab0a9d74773cf74b97cec500e9f48cdab0df31977733a7ceea68e4eacb265e8e2eb8821ef9a684602c5886444620620a9356394642921673aedce99326eaaedaae2e9a735a316adcbcd8c19d9f7de5bd46b8c1dde7d7c56cbe3cbd786a9c6e17d4fe7df47df2b4cf6eb9fcfb85aa8cf4f43ed391dbb8593779a3c40d63addf58f9f7bcd62c29cf73f3cc85b8ef1d52bf9767a29a33dba1efbc57b0ede4b1d19ba70f09af14fcff004eaac93367d2fc1fbbebe39448ef8fcf7953dfcbd9f45beb3af8e7e3bd6f81e7eac9e8f93eaf9fa7ac417a7e666f9dfacf1fc7d96e9c5e833dfda4ab3d1f32df99fd03e75cbd155aede5eda736cc7714c66f5ca0af8a572b9b79d5d28df20e7f55d766371d0f1d97c9a80cfd132ea85e3cdd71d3af3c84f3edcdcadf97b7cbe9dd0397d0973fa3c3df9fabaf8dd4cf9d819fab5d0ebdfcc7cedd8b7e3a6dae9e9ca73874a6f24adbe74c15e8a75c89c6c6a10baa4826ae1003222440a6d31964658d95cd6db289e7a145b1b9b5a25d78864e06a3dc6ca2cd73bf2c2673adb6735cff001debbc9e7a7a3f57c6d3ae7b6b8e1b3c8e3efe2e7e8f7373874f35be2fd87cf73d31c6f8e7a7acf47cdd9d3859c2ecf93978562972f55fa71ebc76ab06fa359f51e8b99b3b78afe3753cecd79ab3651c3e8531e85276fd372ba1e8f9d6f2fa1c35f27e879be9b97abb254fb782af2ddae4797e867f67e7bd16f16159dfc5e4b89d2cfc3ea67f59c1f5d79ef2a3bfcee7790f4dc0f37d18faff002dedf7cf33d15f4f2f81c6d72f6c827356d868e7d70db64ee813cfae38f4e7d78e8ba8d9ae7a4473fa0d05802146c4cf367aabdf8b409e7db0e177706fc183bf8fa0da1ae7efc31cf775f8b0c17e6e9c223b358b7567b39f77ab9fa9b866be8d61db5db34a9ba8b98464b5c62a4843083458da9adb09d72c651924a51736af2fcef3c75e6489be99acfd5e7f52cf5d0e44ee3ab1c105dd2e59673f9b38e3b7bc9f0e7be3daf2bbf839dece871fad9ebdf9f0a1d3cfd6f03dce3e3b3b25a73d3da1c33af97b7e0fd079fcf6cd2d2b9f77a6bd38ddd83a6e63bc6197a3c7b381d1c3cbb155e79fd0b97bacddefcb9f3f57836f175e0e7d73fa4e4686ba473976f3ac1bace5e8b36f35ef8f46ac14dbc7d3a9f93dd3ee707775f26f30bebc79fcbec55e3f73eff0df7e1dbc1933ea722bd93e5ece7dda5192e9856e56ce943ba1374e6d3474e19b4d2ae7a064967d1a4c81accf35b6baa9b8d3662db39b35d39ed9f36bcfaf26b5253aaa3365e8ab4e6b77f3eaaafaf59aac45cdb2829b52addccc5368b22f3d234db5eb9c53579a85815932cac009c5ad901cb1900ecaec9abdd73ceea8b95ce9bf0eac6e990a6a76d24d69aa11a84631d739db52b0957297bfd9f29a758f4479c8194a4c76968cba0a6dcd3b993a59344659ca92b5598edceb5baae9735d89db74b3a3640a5753ae32ee960b73ad308c2990aab4f6fce6dd73f48700df0eb709e5c7a2f8d267a6855116cab996c5195d074c5aeb855aaa2c84aa2e6f21735915a5cbdd86ec5beb2a8ae99e7e98b144ab2b51493ad96dd96d95556c12be861e846ca486730cd7e5dc96de2752f38f2fb1cbd4a2ca5ef1756258384ae74ab6cc74c238ef9d92aa53539562ce0d226ec2a5a2a5a865c5202486965646c9aa9348edaa4b275359b8db2c67522e55b</t>
   </si>
   <si>
-    <t>2019-10-04 00:08:00+07</t>
-  </si>
-  <si>
-    <t>2019-10-04 00:11:30+07</t>
-  </si>
-  <si>
     <t>2020-10-10 00:00:00+07</t>
   </si>
   <si>
-    <t>2019-10-04 00:06:00+07</t>
-  </si>
-  <si>
-    <t>2019-10-04 00:09:00+07</t>
-  </si>
-  <si>
-    <t>2019-10-04 00:07:00+07</t>
-  </si>
-  <si>
-    <t>2019-10-04 00:10:00+07</t>
+    <t>2019-10-04 08:00:00+07</t>
+  </si>
+  <si>
+    <t>2019-10-04 09:30:00+07</t>
+  </si>
+  <si>
+    <t>2019-10-04 00:00:00+07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1
+</t>
+  </si>
+  <si>
+    <t>2019-10-04 07:00:00+07</t>
+  </si>
+  <si>
+    <t>2019-10-04 09:00:00+07</t>
+  </si>
+  <si>
+    <t>2019-10-04 06:30:00+07</t>
+  </si>
+  <si>
+    <t>2019-10-04 11:03:00+07</t>
+  </si>
+  <si>
+    <t>2019-10-04 12:00:00+07</t>
+  </si>
+  <si>
+    <t>createAt</t>
+  </si>
+  <si>
+    <t>updateAt</t>
+  </si>
+  <si>
+    <t>BHD Star - Bitexco</t>
+  </si>
+  <si>
+    <t>Tầng 3 và 4 Tòa nhà tài chính Bitexco, 2 Hải Triều, Bến Nghé, Quận 1, Thành phố Hồ Chí Minh 12345</t>
+  </si>
+  <si>
+    <t>BHD Star - Thảo Điền</t>
+  </si>
+  <si>
+    <t>Tầng 5, TTTM Vincom Mega Mall, 159 Xa lộ Hà Nội, Thảo Điền, Quận 2, Thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>BHD Star - 3/2</t>
+  </si>
+  <si>
+    <t>3 Đường 3/2, Phường 11, Quận 10, Thành phố Hồ Chí Minh 700000</t>
+  </si>
+  <si>
+    <t>BHD Star - Quang Trung</t>
+  </si>
+  <si>
+    <t>190 Quang Trung, Phường 10, Gò Vấp, Thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>CGV - Vạn Hạnh Mail</t>
+  </si>
+  <si>
+    <t>Tầng 6, Vạn Hạnh Mall, 11 Sư Vạn Hạnh, Phường 12, Quận 10, Thành phố Hồ Chí Minh 700000</t>
+  </si>
+  <si>
+    <t>CGV - Thảo Điền</t>
+  </si>
+  <si>
+    <t>12 Đ. Quốc Hương, Thảo Điền, Quận 2, Thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>CGV - 3/2</t>
+  </si>
+  <si>
+    <t>304A Quang Trung, Phường 11, Gò Vấp, Thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>CGV - Quang Trung</t>
+  </si>
+  <si>
+    <t>Beta Cinemas - Quang Trung</t>
+  </si>
+  <si>
+    <t>645 Quang Trung, Phường 11, Gò Vấp, Thành phố Hồ Chí Minh 71421</t>
+  </si>
+  <si>
+    <t>BHD</t>
+  </si>
+  <si>
+    <t>CGV</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Cinestar</t>
   </si>
 </sst>
 </file>
@@ -258,7 +268,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,6 +278,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -461,6 +477,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -778,7 +804,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -804,10 +830,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -815,10 +841,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -826,10 +852,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -837,10 +863,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -848,10 +874,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -859,10 +885,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -870,10 +896,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -881,10 +907,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -892,10 +918,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -906,96 +932,144 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61248DD9-F9F0-421C-9BAE-BA615B0E511A}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="19.375" customWidth="1"/>
     <col min="5" max="5" width="14.125" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="23.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="32">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="32">
+        <v>1</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="32">
+        <v>150</v>
+      </c>
+      <c r="F2" s="32">
+        <v>150</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="32">
+        <v>2</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="32">
+        <v>2</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="32">
+        <v>150</v>
+      </c>
+      <c r="F3" s="32">
+        <v>150</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="32">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="5">
+      <c r="B4" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="32">
+        <v>3</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="32">
         <v>150</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F4" s="32">
         <v>150</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="5">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="G4" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="32">
+        <v>4</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="32">
+        <v>4</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="32">
         <v>150</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F5" s="32">
         <v>150</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="8">
-        <v>1</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="8">
-        <v>150</v>
-      </c>
-      <c r="F4" s="9">
-        <v>150</v>
+      <c r="G5" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1040,16 +1114,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C2" s="17">
         <v>44533</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1057,16 +1131,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -1074,16 +1148,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1093,170 +1167,290 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3FCF28D-9F6E-4A4C-92F3-69FC47D8BA3F}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.25" customWidth="1"/>
     <col min="3" max="3" width="13.125" customWidth="1"/>
-    <col min="5" max="5" width="23.25" customWidth="1"/>
+    <col min="4" max="4" width="14.625" customWidth="1"/>
+    <col min="5" max="5" width="26.25" customWidth="1"/>
+    <col min="6" max="6" width="21.125" customWidth="1"/>
+    <col min="8" max="8" width="25.75" customWidth="1"/>
+    <col min="9" max="9" width="26.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C6" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D6" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G6" s="29" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="21">
-        <v>1</v>
-      </c>
-      <c r="B2" s="22">
-        <v>1</v>
-      </c>
-      <c r="C2" s="22">
-        <v>1</v>
-      </c>
-      <c r="D2" s="23">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="E2" s="23">
-        <v>0.97916666666666663</v>
-      </c>
-      <c r="F2" s="24">
+      <c r="H6" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="30">
+        <v>1</v>
+      </c>
+      <c r="B7" s="30">
+        <v>1</v>
+      </c>
+      <c r="C7" s="30">
+        <v>1</v>
+      </c>
+      <c r="D7" s="30">
+        <v>1</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="30">
         <v>70000</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="21">
+      <c r="H7" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="30">
         <v>2</v>
       </c>
-      <c r="B3" s="22">
-        <v>1</v>
-      </c>
-      <c r="C3" s="22">
+      <c r="B8" s="30">
+        <v>1</v>
+      </c>
+      <c r="C8" s="30">
+        <v>1</v>
+      </c>
+      <c r="D8" s="30">
         <v>2</v>
       </c>
-      <c r="D3" s="23">
-        <v>0.75</v>
-      </c>
-      <c r="E3" s="23">
-        <v>0.875</v>
-      </c>
-      <c r="F3" s="24">
+      <c r="E8" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="30">
         <v>70000</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25">
+      <c r="H8" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="30">
         <v>3</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B9" s="30">
+        <v>1</v>
+      </c>
+      <c r="C9" s="30">
+        <v>1</v>
+      </c>
+      <c r="D9" s="30">
+        <v>1</v>
+      </c>
+      <c r="E9" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="30">
+        <v>70000</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="30">
+        <v>4</v>
+      </c>
+      <c r="B10" s="30">
         <v>2</v>
       </c>
-      <c r="C4" s="26">
-        <v>3</v>
-      </c>
-      <c r="D4" s="27">
-        <v>0.79166666666666696</v>
-      </c>
-      <c r="E4" s="27">
-        <v>0.91666666666666696</v>
-      </c>
-      <c r="F4" s="28">
+      <c r="C10" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="30">
+        <v>2</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="30">
         <v>70000</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10">
+      <c r="H10" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="30">
+        <v>5</v>
+      </c>
+      <c r="B11" s="30">
+        <v>2</v>
+      </c>
+      <c r="C11" s="30">
+        <v>2</v>
+      </c>
+      <c r="D11" s="30">
+        <v>7</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="30">
         <v>70000</v>
       </c>
-      <c r="G10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="H11" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="30">
+        <v>6</v>
+      </c>
+      <c r="B12" s="30">
+        <v>1</v>
+      </c>
+      <c r="C12" s="30">
         <v>2</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
+      <c r="D12" s="30">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11">
+      <c r="E12" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="30">
         <v>70000</v>
       </c>
-      <c r="G11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12">
+      <c r="H12" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="30">
+        <v>7</v>
+      </c>
+      <c r="B13" s="30">
+        <v>1</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="30">
         <v>2</v>
       </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12">
+      <c r="E13" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="30">
         <v>70000</v>
       </c>
-      <c r="G12" t="s">
-        <v>63</v>
+      <c r="H13" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="30" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
done theater theaterCluster movie in admin (showtime and QLDT not )
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Exercises\LTWeb2\Đồ Án Cuối Kỳ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65556622-03B1-43A4-8BFD-A0E1D8275561}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D225F6-E45B-4DEF-AD7A-F21F61DB540B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" activeTab="1" xr2:uid="{EFC861EB-62D1-4F27-80DA-EEC53D8209EB}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" tabRatio="639" firstSheet="1" activeTab="6" xr2:uid="{EFC861EB-62D1-4F27-80DA-EEC53D8209EB}"/>
   </bookViews>
   <sheets>
     <sheet name="TheaterCluster" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="150">
   <si>
     <t>id</t>
   </si>
@@ -76,9 +76,6 @@
   </si>
   <si>
     <t>price</t>
-  </si>
-  <si>
-    <t>userId</t>
   </si>
   <si>
     <t>showTimeId</t>
@@ -245,6 +242,246 @@
   </si>
   <si>
     <t>Cinestar</t>
+  </si>
+  <si>
+    <t>2021-06-13 16:28:28+07</t>
+  </si>
+  <si>
+    <t>2021-06-13 16:28:28.154+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 10:28:20+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 10:28:20.956+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 14:37:41+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 14:37:41.766+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 14:40:50+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 14:40:50.943+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 14:40:51+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 14:40:51.094+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 14:43:44+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 14:43:44.105+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 14:56:14+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 14:56:14.802+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 21:11:59+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 21:11:59.527+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 21:13:12+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 21:13:12.631+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 21:13:35+07</t>
+  </si>
+  <si>
+    <t>2021-06-14 21:13:35.091+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 14:51:25+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 14:51:25.094+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 14:53:14+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 14:53:14.865+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 14:54:24+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 14:54:24.303+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 14:55:16+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 14:55:16.819+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 14:55:44+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 14:55:44.259+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 14:55:54+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 14:55:54.575+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 15:05:24+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 15:05:24.162+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 15:06:42+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 15:06:42.998+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 15:06:55+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 15:06:55.022+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 15:09:18+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 15:09:18.294+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 15:18:49+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 15:18:49.864+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 15:19:18+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 15:19:18.369+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 16:37:28+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 16:37:28.104+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 17:34:03+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 17:34:03.63+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 17:47:08+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 17:47:08.9+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 17:48:16+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 17:48:16.164+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 17:50:04+07</t>
+  </si>
+  <si>
+    <t>2021-06-17 17:50:04.925+07</t>
+  </si>
+  <si>
+    <t>2021-06-18 15:14:19+07</t>
+  </si>
+  <si>
+    <t>2021-06-18 15:14:19.424+07</t>
+  </si>
+  <si>
+    <t>createat</t>
+  </si>
+  <si>
+    <t>crea</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>trailer</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=jluSu8Rw6YE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=odM92ap8_c0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=kBY2k3G6LsM</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bố già là câu chuyện thường nhật về một gia đình ở một xóm lao động nghèo tại thành phố Hồ Chí Minh, ở đó có bộ tứ anh em Giàu, Sang, Phú, Quý. Ba Sang  là cha đơn thân, một mình nuôi hai con Quắn và Bù Tọt, trong đó đứa con trai đầu hơn 20 tuổi tên Quắn là một YouTuber kiếm tiền từ những lượt xem trên YouTube. </t>
+  </si>
+  <si>
+    <t>Năm năm sau khi Godzilla giết kẻ thù ngoài Trái Đất Ghidorah, Godzilla và Kong hiện là những Titan cuối cùng còn hoạt động trên bề mặt Trái Đất nếu không kể Rodan. Ở Đảo Đầu Lâu, khí hậu đã mất ổn định ,cơn bão ở ngoài đảo đã đi chuyển vào trong đảo ,giết tất cả người Iwi. Giờ đây, Monarch theo dõi Kong, kẻ đang cư trú trong một mái vòm khổng lồ. Kong được thăm bởi Jia</t>
+  </si>
+  <si>
+    <t>Lật Mặt 5: 48H là cuộc rượt đuổi, truy lùng của băng nhóm tội phạm để giành lại báu vật quý hiếm . Phim kể về Hiền  - một cựu vận động viên võ thuật sau khi giải nghệ vì chấn thương đã cùng vợ và con gái về quê thăm gia đình Lâm . Họ bị cuốn vào một cuộc rượt đuổi với tay phản diện A Dìn</t>
+  </si>
+  <si>
+    <t>TheaterClisterId</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3295.9063292941596!2d106.70460157431474!3d10.77179242171387!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x31752fae3ea605ab%3A0x2afaf7f3826e5c42!2sBHD%20Star%20Cineplex!5e0!3m2!1sen!2s!4v1623577302425!5m2!1sen!2s" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3919.114183862981!2d106.73940701526037!3d10.802565911663407!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x317526115cf166fb%3A0x6fd050f19935f977!2sBHD%20STAR%20THAO%20DIEN!5e0!3m2!1sen!2s!4v1623577489438!5m2!1sen!2s" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d7839.048313042453!2d106.66728877615155!3d10.771108609132794!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x31752f2661403577%3A0x9257956110ab20c!2sBHD%20Star%20Cineplex!5e0!3m2!1sen!2s!4v1623577532045!5m2!1sen!2s" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m14!1m8!1m3!1d15675.055816954946!2d106.6723785!3d10.8293676!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x0%3A0x8efa606916f6f5f0!2sBHD%20Star%20Cineplex!5e0!3m2!1sen!2s!4v1623577601901!5m2!1sen!2s" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3919.5313393164406!2d106.66735301526028!3d10.77055666224609!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x31752edde029b133%3A0x97e90e1306ccf98e!2zQ0dWIFbhuqFuIEjhuqFuaCBNYWxs!5e0!3m2!1sen!2s!4v1623577625790!5m2!1sen!2s" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3919.125588415216!2d106.73078161526047!3d10.801692061679432!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x3175261a4e5b1ae5%3A0xfa9a912a9c136a45!2zQ0dWIFRo4bqjbyDEkGnhu4FuIFBlYXJs!5e0!3m2!1sen!2s!4v1623577649373!5m2!1sen!2s" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d15677.852627111966!2d106.67168833478873!3d10.7757948808319!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x0%3A0x9ba2ed64e9e3ef7b!2zQ0dWIFZpbmNvbSDEkOG7k25nIEto4bufaQ!5e0!3m2!1sen!2s!4v1623577691485!5m2!1sen!2s" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d62699.0762901071!2d106.63595938230308!3d10.834845377807174!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x0%3A0x6b75d60918c5fc05!2zQ0dWIEfDsiBW4bqlcA!5e0!3m2!1sen!2s!4v1623577753277!5m2!1sen!2s" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m14!1m8!1m3!1d15674.745545566!2d106.6604232!3d10.8352947!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x0%3A0xb68e965b82eea035!2sR%E1%BA%A1p%20phim%20Beta%20Cinemas%20Quang%20Trung!5e0!3m2!1sen!2s!4v1623577779866!5m2!1sen!2s" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3919.3744067046764!2d106.69596251526028!3d10.78260946202688!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x31752f366a781d37%3A0x1f5346650cf7ceb8!2sCinestar%20Hai%20Ba%20Trung!5e0!3m2!1sen!2s!4v1623577798517!5m2!1sen!2s" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>&lt;iframe src="https://www.google.com/maps/embed?pb=!1m18!1m12!1m3!1d3919.618598715473!2d106.68516021526018!3d10.763849162367894!2m3!1f0!2f0!3f0!3m2!1i1024!2i768!4f13.1!3m3!1m2!1s0x31752f19e63f0a05%3A0xd4c41b784ebcc3e8!2sCinestar%20Cinema%20Qu%E1%BB%91c%20Thanh!5e0!3m2!1sen!2s!4v1623577818182!5m2!1sen!2s" width="600" height="450" style="border:0;" allowfullscreen="" loading="lazy"&gt;&lt;/iframe&gt;</t>
+  </si>
+  <si>
+    <t>position</t>
   </si>
 </sst>
 </file>
@@ -288,7 +525,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -405,11 +642,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -487,6 +733,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C7B19E-BBF4-41FD-9065-17500C791EEF}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -812,9 +1065,11 @@
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="28.5" customWidth="1"/>
     <col min="3" max="3" width="110.25" customWidth="1"/>
+    <col min="4" max="4" width="17.75" customWidth="1"/>
+    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -824,104 +1079,177 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>66</v>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -934,7 +1262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61248DD9-F9F0-421C-9BAE-BA615B0E511A}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -973,13 +1301,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="32">
         <v>1</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="32">
         <v>150</v>
@@ -988,10 +1316,10 @@
         <v>150</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -999,13 +1327,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="32">
         <v>2</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="32">
         <v>150</v>
@@ -1014,10 +1342,10 @@
         <v>150</v>
       </c>
       <c r="G3" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1025,13 +1353,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="32">
         <v>3</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="32">
         <v>150</v>
@@ -1040,10 +1368,10 @@
         <v>150</v>
       </c>
       <c r="G4" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1051,13 +1379,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="32">
         <v>4</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="32">
         <v>150</v>
@@ -1066,10 +1394,10 @@
         <v>150</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H5" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1079,10 +1407,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298BA02F-AA7E-434E-AD22-C44EF0C96355}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1092,7 +1420,7 @@
     <col min="4" max="4" width="32.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -1103,61 +1431,85 @@
         <v>7</v>
       </c>
       <c r="D1" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="17">
         <v>44533</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D2" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>2</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="11" t="s">
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13">
-        <v>3</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="G4" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1169,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3FCF28D-9F6E-4A4C-92F3-69FC47D8BA3F}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1239,10 +1591,10 @@
         <v>14</v>
       </c>
       <c r="H6" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="29" t="s">
         <v>48</v>
-      </c>
-      <c r="I6" s="29" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1259,19 +1611,19 @@
         <v>1</v>
       </c>
       <c r="E7" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="30" t="s">
         <v>39</v>
-      </c>
-      <c r="F7" s="30" t="s">
-        <v>40</v>
       </c>
       <c r="G7" s="30">
         <v>70000</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1288,19 +1640,19 @@
         <v>2</v>
       </c>
       <c r="E8" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="30" t="s">
         <v>39</v>
-      </c>
-      <c r="F8" s="30" t="s">
-        <v>40</v>
       </c>
       <c r="G8" s="30">
         <v>70000</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1317,19 +1669,19 @@
         <v>1</v>
       </c>
       <c r="E9" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="30" t="s">
         <v>39</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>40</v>
       </c>
       <c r="G9" s="30">
         <v>70000</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I9" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
@@ -1340,25 +1692,25 @@
         <v>2</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="30">
         <v>2</v>
       </c>
       <c r="E10" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="30" t="s">
         <v>43</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>44</v>
       </c>
       <c r="G10" s="30">
         <v>70000</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I10" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1375,19 +1727,19 @@
         <v>7</v>
       </c>
       <c r="E11" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="30" t="s">
         <v>43</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>44</v>
       </c>
       <c r="G11" s="30">
         <v>70000</v>
       </c>
       <c r="H11" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I11" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1404,19 +1756,19 @@
         <v>2</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" s="30">
         <v>70000</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I12" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
@@ -1427,25 +1779,25 @@
         <v>1</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="30">
         <v>2</v>
       </c>
       <c r="E13" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="30" t="s">
         <v>46</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>47</v>
       </c>
       <c r="G13" s="30">
         <v>70000</v>
       </c>
       <c r="H13" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I13" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1456,19 +1808,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7910DE4F-508C-467C-9C59-946A7F25DAFC}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="30.625" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
+    <col min="5" max="5" width="26.125" customWidth="1"/>
+    <col min="6" max="6" width="25.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1476,13 +1831,663 @@
         <v>15</v>
       </c>
       <c r="C1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="F1" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>140000</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>210000</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>210000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>280000</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>280000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>210000</v>
+      </c>
+      <c r="F7" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>210000</v>
+      </c>
+      <c r="F8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>140000</v>
+      </c>
+      <c r="F9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>140000</v>
+      </c>
+      <c r="F10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>140000</v>
+      </c>
+      <c r="F11" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>70000</v>
+      </c>
+      <c r="F12" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>70000</v>
+      </c>
+      <c r="F13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>70000</v>
+      </c>
+      <c r="F14" t="s">
+        <v>95</v>
+      </c>
+      <c r="G14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>210000</v>
+      </c>
+      <c r="F15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>140000</v>
+      </c>
+      <c r="F16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>70000</v>
+      </c>
+      <c r="F17" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>17</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>70000</v>
+      </c>
+      <c r="F18" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>70000</v>
+      </c>
+      <c r="F19" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>70000</v>
+      </c>
+      <c r="F20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>70000</v>
+      </c>
+      <c r="F21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>70000</v>
+      </c>
+      <c r="F22" t="s">
+        <v>111</v>
+      </c>
+      <c r="G22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>70000</v>
+      </c>
+      <c r="F23" t="s">
+        <v>113</v>
+      </c>
+      <c r="G23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>140000</v>
+      </c>
+      <c r="F24" t="s">
+        <v>115</v>
+      </c>
+      <c r="G24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>140000</v>
+      </c>
+      <c r="F25" t="s">
+        <v>117</v>
+      </c>
+      <c r="G25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>70000</v>
+      </c>
+      <c r="F26" t="s">
+        <v>119</v>
+      </c>
+      <c r="G26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>70000</v>
+      </c>
+      <c r="F27" t="s">
+        <v>121</v>
+      </c>
+      <c r="G27" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>122</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>70000</v>
+      </c>
+      <c r="F28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>210000</v>
+      </c>
+      <c r="F29" t="s">
+        <v>125</v>
+      </c>
+      <c r="G29" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1509,10 +2514,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>19</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>14</v>
@@ -1525,10 +2530,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A232FC14-E6D1-49DD-9B16-FDAD383530E4}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1537,27 +2542,30 @@
     <col min="4" max="4" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="G1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="19" t="s">
-        <v>25</v>
+      <c r="H1" s="35" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>